<commit_message>
added decision_metrics to the end of the analysis
</commit_message>
<xml_diff>
--- a/code/Screener/record.xlsx
+++ b/code/Screener/record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAC52005-401D-4774-9127-7C0CBDEC3716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DF5A97-431F-4F99-9669-5F4F101AA1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-18120" windowWidth="28110" windowHeight="18240" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
@@ -45,6 +45,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3329,7 +3351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3379,9 +3401,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3392,9 +3411,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -3404,6 +3420,13 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3446,7 +3469,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{800A4AE0-8832-82D1-6FCB-13DE068DAB5D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3507,7 +3530,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEACA21A-1A8F-8F7C-3B57-145588D9A99D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3573,7 +3596,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{384AACC3-18A5-297F-81C8-08C85D6F790F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3634,7 +3657,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1C9BB9E-9C8C-0BD3-34B3-C197CD43EBED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3700,7 +3723,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BA4DC29-5CFF-7C26-7818-7936808786E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3761,7 +3784,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2131B327-1994-B889-4AFE-8FF23FC59AC2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3822,7 +3845,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60E8078E-5BF8-4E90-7F6A-BC83B93E3849}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3888,7 +3911,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23B7348A-504D-C559-446F-21DCF71169C6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3949,7 +3972,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D25518B4-23B7-C3D4-012D-735A2C041586}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4015,7 +4038,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BDD1587-939C-34C0-0953-D4FBA81D1DAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4076,7 +4099,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0AACDC2-ADB1-2DA4-11F4-A37C8EA16722}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4142,7 +4165,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DF96C57-6C97-88E3-1AB7-6C715EB7F16C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4203,7 +4226,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E4D639E-2F2C-944A-E325-4B3509DEAC9C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4269,7 +4292,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A09BEDF-E02C-9991-E3A4-24B40A8E5D87}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4330,7 +4353,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0FE7D88-4CB3-8385-C8BC-23D7EEDC5346}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4396,7 +4419,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{861BDBF1-C1CD-E54D-DD67-06EE24263B24}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4457,7 +4480,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B876998-2903-0012-9311-CE8D81BA637C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4523,7 +4546,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD92BB1D-EB6C-CBA4-447E-9EB43B4CD366}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4584,7 +4607,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BE9B09F-4EC6-22EF-3046-E4BF4C5AF9E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4650,7 +4673,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7A40239-A4C2-2485-39C3-7175A25B91BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4711,7 +4734,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC97946E-BFDE-EB49-79F2-7246F38FC159}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4777,7 +4800,7 @@
                   <a14:compatExt spid="_x0000_s10243"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09C1BFAA-8BC5-F43B-6A8F-CA1681FA0938}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003280000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4827,7 +4850,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89D6DEC3-40CF-AD93-D5BB-3C8A2329FAF4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4888,7 +4911,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E4EA3D4-5686-AE0C-365F-5837C83833C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4954,7 +4977,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66484773-2BDC-5D97-F537-256C2AF81800}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5015,7 +5038,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CE6F07F-78F6-20FE-F15B-B820A2BDDB09}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5081,7 +5104,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D5916FE-F90B-4D84-D381-D4D1286424E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5142,7 +5165,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE740E01-83CC-6FC0-A477-EEC7EF4D6006}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5485,45 +5508,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EC1B12-8D19-48E1-AE18-CC4CE60CD15C}">
-  <dimension ref="B9:P51"/>
+  <dimension ref="B9:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="19"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="2:16">
-      <c r="I9">
-        <f>SUM(I11:I49)</f>
-        <v>-25252</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" ht="77.25">
-      <c r="J10" t="s">
+    <row r="9" spans="2:17">
+      <c r="H9" s="19"/>
+      <c r="J9">
+        <f>SUM(J11:J49)</f>
+        <v>-25784.559999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="77.25">
+      <c r="K10" t="s">
         <v>11</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>190</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="M10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="N10" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>416</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="2:17">
       <c r="B11" s="1">
         <v>44714</v>
       </c>
@@ -5536,35 +5561,39 @@
       <c r="E11">
         <v>102</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="19" cm="1">
+        <f t="array" ref="F11">SUMPRODUCT(($C$11:$C$51=C11)*($E$11:$E$51))</f>
+        <v>0</v>
+      </c>
+      <c r="G11">
         <v>48.99</v>
       </c>
-      <c r="G11">
-        <f t="shared" ref="G11:G18" si="0">F11*E11</f>
+      <c r="H11">
+        <f t="shared" ref="H11:H18" si="0">G11*E11</f>
         <v>4996.9800000000005</v>
       </c>
-      <c r="H11">
-        <f t="shared" ref="H11:H18" si="1">IF(D11="Buy",-1,1)</f>
+      <c r="I11">
+        <f t="shared" ref="I11:I18" si="1">IF(D11="Buy",-1,1)</f>
         <v>-1</v>
       </c>
-      <c r="I11">
-        <f t="shared" ref="I11:I18" si="2">H11*G11</f>
+      <c r="J11">
+        <f t="shared" ref="J11:J18" si="2">I11*H11</f>
         <v>-4996.9800000000005</v>
       </c>
-      <c r="N11">
-        <f>AVERAGE(N26:N32)</f>
+      <c r="O11">
+        <f>AVERAGE(O26:O32)</f>
         <v>78.400000000000006</v>
       </c>
-      <c r="O11" s="16">
-        <f>AVERAGE(O26:O60)</f>
+      <c r="P11" s="16">
+        <f>AVERAGE(P26:P60)</f>
         <v>2.1790212754845828E-3</v>
       </c>
-      <c r="P11" s="16">
-        <f>(1+O11)^92</f>
+      <c r="Q11" s="16">
+        <f>(1+P11)^92</f>
         <v>1.2217104193544945</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="2:17">
       <c r="B12" s="1">
         <v>44714</v>
       </c>
@@ -5577,23 +5606,27 @@
       <c r="E12">
         <v>16</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="19" cm="1">
+        <f t="array" ref="F12">SUMPRODUCT(($C$11:$C$51=C12)*($E$11:$E$51))</f>
+        <v>6</v>
+      </c>
+      <c r="G12">
         <v>318.58</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="0"/>
         <v>5097.28</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <f t="shared" si="2"/>
         <v>-5097.28</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:17">
       <c r="B13" s="1">
         <v>44717</v>
       </c>
@@ -5604,25 +5637,28 @@
         <v>3</v>
       </c>
       <c r="E13">
-        <v>102</v>
-      </c>
-      <c r="F13">
+        <v>-102</v>
+      </c>
+      <c r="F13" s="19" cm="1">
+        <f t="array" ref="F13">SUMPRODUCT(($C$11:$C$51=C13)*($E$11:$E$51))</f>
+        <v>0</v>
+      </c>
+      <c r="G13">
         <v>48.26</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="0"/>
-        <v>4922.5199999999995</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-4922.5199999999995</v>
       </c>
       <c r="I13">
+        <v>-1</v>
+      </c>
+      <c r="J13">
         <f t="shared" si="2"/>
         <v>4922.5199999999995</v>
       </c>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="2:17">
       <c r="B14" s="1">
         <v>44717</v>
       </c>
@@ -5633,25 +5669,28 @@
         <v>3</v>
       </c>
       <c r="E14">
-        <v>16</v>
-      </c>
-      <c r="F14">
+        <v>-16</v>
+      </c>
+      <c r="F14" s="19" cm="1">
+        <f t="array" ref="F14">SUMPRODUCT(($C$11:$C$51=C14)*($E$11:$E$51))</f>
+        <v>6</v>
+      </c>
+      <c r="G14">
         <v>313.27</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="0"/>
-        <v>5012.32</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I14">
+        <v>-5012.32</v>
+      </c>
+      <c r="I14" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J14">
         <f t="shared" si="2"/>
         <v>5012.32</v>
       </c>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="2:17">
       <c r="B15" s="1">
         <v>44719</v>
       </c>
@@ -5664,23 +5703,26 @@
       <c r="E15">
         <v>6</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="19" cm="1">
+        <f t="array" ref="F15">SUMPRODUCT(($C$11:$C$51=C15)*($E$11:$E$51))</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
         <v>178.03</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>1068.18</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="1"/>
+      <c r="I15" s="19">
         <v>-1</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <f t="shared" si="2"/>
         <v>-1068.18</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:17">
       <c r="B16" s="1">
         <v>44719</v>
       </c>
@@ -5693,23 +5735,26 @@
       <c r="E16">
         <v>9</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="19" cm="1">
+        <f t="array" ref="F16">SUMPRODUCT(($C$11:$C$51=C16)*($E$11:$E$51))</f>
+        <v>9</v>
+      </c>
+      <c r="G16">
         <v>109.92</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>989.28</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="1"/>
+      <c r="I16" s="19">
         <v>-1</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <f t="shared" si="2"/>
         <v>-989.28</v>
       </c>
     </row>
-    <row r="17" spans="2:16">
+    <row r="17" spans="2:17">
       <c r="B17" s="1">
         <v>44719</v>
       </c>
@@ -5722,23 +5767,26 @@
       <c r="E17">
         <v>9</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="19" cm="1">
+        <f t="array" ref="F17">SUMPRODUCT(($C$11:$C$51=C17)*($E$11:$E$51))</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
         <v>122.55</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>1102.95</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="1"/>
+      <c r="I17" s="19">
         <v>-1</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <f t="shared" si="2"/>
         <v>-1102.95</v>
       </c>
     </row>
-    <row r="18" spans="2:16">
+    <row r="18" spans="2:17">
       <c r="B18" s="1">
         <v>44720</v>
       </c>
@@ -5751,23 +5799,26 @@
       <c r="E18">
         <v>9</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="19" cm="1">
+        <f t="array" ref="F18">SUMPRODUCT(($C$11:$C$51=C18)*($E$11:$E$51))</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
         <v>103.21</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>928.89</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="1"/>
+      <c r="I18" s="19">
         <v>-1</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <f t="shared" si="2"/>
         <v>-928.89</v>
       </c>
     </row>
-    <row r="19" spans="2:16">
+    <row r="19" spans="2:17">
       <c r="B19" s="1">
         <v>44720</v>
       </c>
@@ -5778,25 +5829,28 @@
         <v>3</v>
       </c>
       <c r="E19">
-        <v>9</v>
-      </c>
-      <c r="F19">
+        <v>-9</v>
+      </c>
+      <c r="F19" s="19" cm="1">
+        <f t="array" ref="F19">SUMPRODUCT(($C$11:$C$51=C19)*($E$11:$E$51))</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
         <v>103.5</v>
       </c>
-      <c r="G19">
-        <f t="shared" ref="G19:G27" si="3">F19*E19</f>
+      <c r="H19">
+        <f t="shared" ref="H19:H27" si="3">G19*E19</f>
+        <v>-931.5</v>
+      </c>
+      <c r="I19" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J19">
+        <f t="shared" ref="J19:J27" si="4">I19*H19</f>
         <v>931.5</v>
       </c>
-      <c r="H19">
-        <f t="shared" ref="H19:H25" si="4">IF(D19="Buy",-1,1)</f>
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <f t="shared" ref="I19:I27" si="5">H19*G19</f>
-        <v>931.5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16">
+    </row>
+    <row r="20" spans="2:17">
       <c r="B20" s="1">
         <v>44719</v>
       </c>
@@ -5807,25 +5861,28 @@
         <v>3</v>
       </c>
       <c r="E20">
+        <v>-9</v>
+      </c>
+      <c r="F20" s="19" cm="1">
+        <f t="array" ref="F20">SUMPRODUCT(($C$11:$C$51=C20)*($E$11:$E$51))</f>
         <v>9</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>111.36</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <f t="shared" si="3"/>
+        <v>-1002.24</v>
+      </c>
+      <c r="I20" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="4"/>
         <v>1002.24</v>
       </c>
-      <c r="H20">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="5"/>
-        <v>1002.24</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16">
+    </row>
+    <row r="21" spans="2:17">
       <c r="B21" s="1">
         <v>44719</v>
       </c>
@@ -5836,25 +5893,28 @@
         <v>3</v>
       </c>
       <c r="E21">
-        <v>9</v>
-      </c>
-      <c r="F21">
+        <v>-9</v>
+      </c>
+      <c r="F21" s="19" cm="1">
+        <f t="array" ref="F21">SUMPRODUCT(($C$11:$C$51=C21)*($E$11:$E$51))</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
         <v>118.56</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <f t="shared" si="3"/>
+        <v>-1067.04</v>
+      </c>
+      <c r="I21" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="4"/>
         <v>1067.04</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="5"/>
-        <v>1067.04</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16">
+    </row>
+    <row r="22" spans="2:17">
       <c r="B22" s="1">
         <v>44720</v>
       </c>
@@ -5865,25 +5925,28 @@
         <v>3</v>
       </c>
       <c r="E22">
-        <v>9</v>
-      </c>
-      <c r="F22">
+        <v>-6</v>
+      </c>
+      <c r="F22" s="19" cm="1">
+        <f t="array" ref="F22">SUMPRODUCT(($C$11:$C$51=C22)*($E$11:$E$51))</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
         <v>177.52</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <f t="shared" si="3"/>
-        <v>1597.68</v>
-      </c>
-      <c r="H22">
+        <v>-1065.1200000000001</v>
+      </c>
+      <c r="I22" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J22">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="5"/>
-        <v>1597.68</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16">
+        <v>1065.1200000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17">
       <c r="B23" s="1">
         <v>44722</v>
       </c>
@@ -5896,23 +5959,26 @@
       <c r="E23">
         <v>20</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="19" cm="1">
+        <f t="array" ref="F23">SUMPRODUCT(($C$11:$C$51=C23)*($E$11:$E$51))</f>
+        <v>41</v>
+      </c>
+      <c r="G23">
         <v>48.94</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <f t="shared" si="3"/>
         <v>978.8</v>
       </c>
-      <c r="H23">
+      <c r="I23" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J23">
         <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="5"/>
         <v>-978.8</v>
       </c>
     </row>
-    <row r="24" spans="2:16">
+    <row r="24" spans="2:17">
       <c r="B24" s="1">
         <v>44723</v>
       </c>
@@ -5925,29 +5991,32 @@
       <c r="E24">
         <v>3</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="19" cm="1">
+        <f t="array" ref="F24">SUMPRODUCT(($C$11:$C$51=C24)*($E$11:$E$51))</f>
+        <v>6</v>
+      </c>
+      <c r="G24">
         <v>305.58999999999997</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <f t="shared" si="3"/>
         <v>916.77</v>
       </c>
-      <c r="H24">
+      <c r="I24" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J24">
         <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="5"/>
         <v>-916.77</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>10</v>
       </c>
-      <c r="L24" s="1">
+      <c r="M24" s="1">
         <v>44763</v>
       </c>
     </row>
-    <row r="25" spans="2:16">
+    <row r="25" spans="2:17">
       <c r="B25" s="1">
         <v>44723</v>
       </c>
@@ -5960,29 +6029,32 @@
       <c r="E25">
         <v>16</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="19" cm="1">
+        <f t="array" ref="F25">SUMPRODUCT(($C$11:$C$51=C25)*($E$11:$E$51))</f>
+        <v>32</v>
+      </c>
+      <c r="G25">
         <v>63.85</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <f t="shared" si="3"/>
         <v>1021.6</v>
       </c>
-      <c r="H25">
+      <c r="I25" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J25">
         <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="5"/>
         <v>-1021.6</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>10</v>
       </c>
-      <c r="L25" s="1">
+      <c r="M25" s="1">
         <v>44749</v>
       </c>
     </row>
-    <row r="26" spans="2:16">
+    <row r="26" spans="2:17">
       <c r="B26" s="1">
         <v>44724</v>
       </c>
@@ -5995,47 +6067,50 @@
       <c r="E26">
         <v>3</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="19" cm="1">
+        <f t="array" ref="F26">SUMPRODUCT(($C$11:$C$51=C26)*($E$11:$E$51))</f>
+        <v>6</v>
+      </c>
+      <c r="G26">
         <v>305.99</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <f t="shared" si="3"/>
         <v>917.97</v>
       </c>
-      <c r="H26">
-        <f t="shared" ref="H26:H43" si="6">IF(D26="Buy",-1,1)</f>
+      <c r="I26" s="19">
         <v>-1</v>
       </c>
-      <c r="I26">
-        <f t="shared" si="5"/>
+      <c r="J26">
+        <f t="shared" si="4"/>
         <v>-917.97</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>10</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>141</v>
       </c>
-      <c r="L26" s="1">
+      <c r="M26" s="1">
         <v>44808</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>0.1</v>
       </c>
-      <c r="N26" s="16">
-        <f>L26-B26</f>
+      <c r="O26" s="16">
+        <f>M26-B26</f>
         <v>84</v>
       </c>
-      <c r="O26" s="16">
-        <f>(1+M26)^(1/N26)-1</f>
+      <c r="P26" s="16">
+        <f>(1+N26)^(1/O26)-1</f>
         <v>1.135288950835589E-3</v>
       </c>
-      <c r="P26" s="16">
-        <f>(1+O26)^92</f>
+      <c r="Q26" s="16">
+        <f>(1+P26)^92</f>
         <v>1.1100303305665855</v>
       </c>
     </row>
-    <row r="27" spans="2:16">
+    <row r="27" spans="2:17">
       <c r="B27" s="1">
         <v>44724</v>
       </c>
@@ -6048,32 +6123,35 @@
       <c r="E27">
         <v>100</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="19" cm="1">
+        <f t="array" ref="F27">SUMPRODUCT(($C$11:$C$51=C27)*($E$11:$E$51))</f>
+        <v>32</v>
+      </c>
+      <c r="G27">
         <v>66.5</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <f t="shared" si="3"/>
         <v>6650</v>
       </c>
-      <c r="H27">
-        <f t="shared" si="6"/>
+      <c r="I27" s="19">
         <v>-1</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="5"/>
+      <c r="J27">
+        <f t="shared" si="4"/>
         <v>-6650</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>10</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>142</v>
       </c>
-      <c r="L27" s="1">
+      <c r="M27" s="1">
         <v>44766</v>
       </c>
     </row>
-    <row r="28" spans="2:16">
+    <row r="28" spans="2:17">
       <c r="B28" s="1">
         <v>44724</v>
       </c>
@@ -6084,34 +6162,37 @@
         <v>3</v>
       </c>
       <c r="E28">
-        <v>100</v>
-      </c>
-      <c r="F28">
+        <v>-100</v>
+      </c>
+      <c r="F28" s="19" cm="1">
+        <f t="array" ref="F28">SUMPRODUCT(($C$11:$C$51=C28)*($E$11:$E$51))</f>
+        <v>32</v>
+      </c>
+      <c r="G28">
         <v>63.75</v>
       </c>
-      <c r="G28">
-        <f t="shared" ref="G28" si="7">F28*E28</f>
+      <c r="H28">
+        <f t="shared" ref="H28" si="5">G28*E28</f>
+        <v>-6375</v>
+      </c>
+      <c r="I28" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J28">
+        <f t="shared" ref="J28" si="6">I28*H28</f>
         <v>6375</v>
       </c>
-      <c r="H28">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="I28">
-        <f t="shared" ref="I28" si="8">H28*G28</f>
-        <v>6375</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>10</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>142</v>
       </c>
-      <c r="L28" s="1">
+      <c r="M28" s="1">
         <v>44766</v>
       </c>
     </row>
-    <row r="29" spans="2:16">
+    <row r="29" spans="2:17">
       <c r="B29" s="1">
         <v>44724</v>
       </c>
@@ -6124,47 +6205,50 @@
       <c r="E29">
         <v>16</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="19" cm="1">
+        <f t="array" ref="F29">SUMPRODUCT(($C$11:$C$51=C29)*($E$11:$E$51))</f>
+        <v>32</v>
+      </c>
+      <c r="G29">
         <v>63.75</v>
       </c>
-      <c r="G29">
-        <f t="shared" ref="G29:G50" si="9">F29*E29</f>
+      <c r="H29">
+        <f t="shared" ref="H29:H50" si="7">G29*E29</f>
         <v>1020</v>
       </c>
-      <c r="H29">
-        <f t="shared" si="6"/>
+      <c r="I29" s="19">
         <v>-1</v>
       </c>
-      <c r="I29">
-        <f t="shared" ref="I29:I43" si="10">H29*G29</f>
+      <c r="J29">
+        <f t="shared" ref="J29:J43" si="8">I29*H29</f>
         <v>-1020</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>10</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>142</v>
       </c>
-      <c r="L29" s="1">
+      <c r="M29" s="1">
         <v>44815</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>0.41</v>
       </c>
-      <c r="N29" s="16">
-        <f>L29-B29</f>
+      <c r="O29" s="16">
+        <f t="shared" ref="O29:O51" si="9">M29-B29</f>
         <v>91</v>
       </c>
-      <c r="O29" s="16">
-        <f>(1+M29)^(1/N29)-1</f>
+      <c r="P29" s="16">
+        <f t="shared" ref="P29:P51" si="10">(1+N29)^(1/O29)-1</f>
         <v>3.7828480137320764E-3</v>
       </c>
-      <c r="P29" s="16">
-        <f>(1+O29)^92</f>
+      <c r="Q29" s="16">
+        <f t="shared" ref="Q29:Q51" si="11">(1+P29)^92</f>
         <v>1.4153338156993678</v>
       </c>
     </row>
-    <row r="30" spans="2:16">
+    <row r="30" spans="2:17">
       <c r="B30" s="1">
         <v>44724</v>
       </c>
@@ -6177,47 +6261,50 @@
       <c r="E30">
         <v>6</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="19" cm="1">
+        <f t="array" ref="F30">SUMPRODUCT(($C$11:$C$51=C30)*($E$11:$E$51))</f>
+        <v>6</v>
+      </c>
+      <c r="G30">
         <v>176.69</v>
       </c>
-      <c r="G30">
+      <c r="H30">
+        <f t="shared" si="7"/>
+        <v>1060.1399999999999</v>
+      </c>
+      <c r="I30" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="8"/>
+        <v>-1060.1399999999999</v>
+      </c>
+      <c r="K30" t="s">
+        <v>112</v>
+      </c>
+      <c r="L30" t="s">
+        <v>163</v>
+      </c>
+      <c r="M30" s="1">
+        <v>44787</v>
+      </c>
+      <c r="N30">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="O30" s="16">
         <f t="shared" si="9"/>
-        <v>1060.1399999999999</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I30">
+        <v>63</v>
+      </c>
+      <c r="P30" s="16">
         <f t="shared" si="10"/>
-        <v>-1060.1399999999999</v>
-      </c>
-      <c r="J30" t="s">
-        <v>112</v>
-      </c>
-      <c r="K30" t="s">
-        <v>163</v>
-      </c>
-      <c r="L30" s="1">
-        <v>44787</v>
-      </c>
-      <c r="M30">
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="N30" s="16">
-        <f>L30-B30</f>
-        <v>63</v>
-      </c>
-      <c r="O30" s="16">
-        <f>(1+M30)^(1/N30)-1</f>
         <v>1.9980443135318993E-3</v>
       </c>
-      <c r="P30" s="16">
-        <f>(1+O30)^92</f>
+      <c r="Q30" s="16">
+        <f t="shared" si="11"/>
         <v>1.2015791869493655</v>
       </c>
     </row>
-    <row r="31" spans="2:16">
+    <row r="31" spans="2:17">
       <c r="B31" s="1">
         <v>44724</v>
       </c>
@@ -6230,47 +6317,50 @@
       <c r="E31">
         <v>12</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="19" cm="1">
+        <f t="array" ref="F31">SUMPRODUCT(($C$11:$C$51=C31)*($E$11:$E$51))</f>
+        <v>12</v>
+      </c>
+      <c r="G31">
         <v>84</v>
       </c>
-      <c r="G31">
+      <c r="H31">
+        <f t="shared" si="7"/>
+        <v>1008</v>
+      </c>
+      <c r="I31" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="8"/>
+        <v>-1008</v>
+      </c>
+      <c r="K31" t="s">
+        <v>415</v>
+      </c>
+      <c r="L31" t="s">
+        <v>142</v>
+      </c>
+      <c r="M31" s="1">
+        <v>44801</v>
+      </c>
+      <c r="N31">
+        <v>0.17</v>
+      </c>
+      <c r="O31" s="16">
         <f t="shared" si="9"/>
-        <v>1008</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I31">
+        <v>77</v>
+      </c>
+      <c r="P31" s="16">
         <f t="shared" si="10"/>
-        <v>-1008</v>
-      </c>
-      <c r="J31" t="s">
-        <v>415</v>
-      </c>
-      <c r="K31" t="s">
-        <v>142</v>
-      </c>
-      <c r="L31" s="1">
-        <v>44801</v>
-      </c>
-      <c r="M31">
-        <v>0.17</v>
-      </c>
-      <c r="N31" s="16">
-        <f>L31-B31</f>
-        <v>77</v>
-      </c>
-      <c r="O31" s="16">
-        <f>(1+M31)^(1/N31)-1</f>
         <v>2.0410899187346399E-3</v>
       </c>
-      <c r="P31" s="16">
-        <f>(1+O31)^92</f>
+      <c r="Q31" s="16">
+        <f t="shared" si="11"/>
         <v>1.2063374816411372</v>
       </c>
     </row>
-    <row r="32" spans="2:16">
+    <row r="32" spans="2:17">
       <c r="B32" s="1">
         <v>44724</v>
       </c>
@@ -6283,47 +6373,50 @@
       <c r="E32">
         <v>9</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="19" cm="1">
+        <f t="array" ref="F32">SUMPRODUCT(($C$11:$C$51=C32)*($E$11:$E$51))</f>
+        <v>9</v>
+      </c>
+      <c r="G32">
         <v>108.34</v>
       </c>
-      <c r="G32">
+      <c r="H32">
+        <f t="shared" si="7"/>
+        <v>975.06000000000006</v>
+      </c>
+      <c r="I32" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="8"/>
+        <v>-975.06000000000006</v>
+      </c>
+      <c r="K32" t="s">
+        <v>415</v>
+      </c>
+      <c r="L32" t="s">
+        <v>142</v>
+      </c>
+      <c r="M32" s="1">
+        <v>44801</v>
+      </c>
+      <c r="N32">
+        <v>0.12</v>
+      </c>
+      <c r="O32" s="16">
         <f t="shared" si="9"/>
-        <v>975.06000000000006</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I32">
+        <v>77</v>
+      </c>
+      <c r="P32" s="16">
         <f t="shared" si="10"/>
-        <v>-975.06000000000006</v>
-      </c>
-      <c r="J32" t="s">
-        <v>415</v>
-      </c>
-      <c r="K32" t="s">
-        <v>142</v>
-      </c>
-      <c r="L32" s="1">
-        <v>44801</v>
-      </c>
-      <c r="M32">
-        <v>0.12</v>
-      </c>
-      <c r="N32" s="16">
-        <f>L32-B32</f>
-        <v>77</v>
-      </c>
-      <c r="O32" s="16">
-        <f>(1+M32)^(1/N32)-1</f>
         <v>1.4728847386982213E-3</v>
       </c>
-      <c r="P32" s="16">
-        <f>(1+O32)^92</f>
+      <c r="Q32" s="16">
+        <f t="shared" si="11"/>
         <v>1.1450012193329568</v>
       </c>
     </row>
-    <row r="33" spans="2:16">
+    <row r="33" spans="2:17">
       <c r="B33" s="1">
         <v>44724</v>
       </c>
@@ -6336,47 +6429,50 @@
       <c r="E33">
         <v>6</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="19" cm="1">
+        <f t="array" ref="F33">SUMPRODUCT(($C$11:$C$51=C33)*($E$11:$E$51))</f>
+        <v>6</v>
+      </c>
+      <c r="G33">
         <v>180.07</v>
       </c>
-      <c r="G33">
+      <c r="H33">
+        <f t="shared" si="7"/>
+        <v>1080.42</v>
+      </c>
+      <c r="I33" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="8"/>
+        <v>-1080.42</v>
+      </c>
+      <c r="K33" t="s">
+        <v>433</v>
+      </c>
+      <c r="L33" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33" s="1">
+        <v>44801</v>
+      </c>
+      <c r="N33">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="O33">
         <f t="shared" si="9"/>
-        <v>1080.42</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I33">
+        <v>77</v>
+      </c>
+      <c r="P33">
         <f t="shared" si="10"/>
-        <v>-1080.42</v>
-      </c>
-      <c r="J33" t="s">
-        <v>433</v>
-      </c>
-      <c r="K33" t="s">
-        <v>11</v>
-      </c>
-      <c r="L33" s="1">
-        <v>44801</v>
-      </c>
-      <c r="M33">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="N33">
-        <f>L33-B33</f>
-        <v>77</v>
-      </c>
-      <c r="O33">
-        <f>(1+M33)^(1/N33)-1</f>
         <v>1.6115046098634789E-3</v>
       </c>
-      <c r="P33">
-        <f>(1+O33)^92</f>
+      <c r="Q33">
+        <f t="shared" si="11"/>
         <v>1.1596741873887326</v>
       </c>
     </row>
-    <row r="34" spans="2:16">
+    <row r="34" spans="2:17">
       <c r="B34" s="1">
         <v>44724</v>
       </c>
@@ -6389,47 +6485,50 @@
       <c r="E34">
         <v>3</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="19" cm="1">
+        <f t="array" ref="F34">SUMPRODUCT(($C$11:$C$51=C34)*($E$11:$E$51))</f>
+        <v>3</v>
+      </c>
+      <c r="G34">
         <v>339.23</v>
       </c>
-      <c r="G34">
+      <c r="H34">
+        <f t="shared" si="7"/>
+        <v>1017.69</v>
+      </c>
+      <c r="I34" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="8"/>
+        <v>-1017.69</v>
+      </c>
+      <c r="K34" t="s">
+        <v>435</v>
+      </c>
+      <c r="L34" t="s">
+        <v>11</v>
+      </c>
+      <c r="M34" s="1">
+        <v>44766</v>
+      </c>
+      <c r="N34">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="O34">
         <f t="shared" si="9"/>
-        <v>1017.69</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I34">
+        <v>42</v>
+      </c>
+      <c r="P34">
         <f t="shared" si="10"/>
-        <v>-1017.69</v>
-      </c>
-      <c r="J34" t="s">
-        <v>435</v>
-      </c>
-      <c r="K34" t="s">
-        <v>11</v>
-      </c>
-      <c r="L34" s="1">
-        <v>44766</v>
-      </c>
-      <c r="M34">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="N34">
-        <f>L34-B34</f>
-        <v>42</v>
-      </c>
-      <c r="O34">
-        <f>(1+M34)^(1/N34)-1</f>
         <v>2.2501629544413593E-3</v>
       </c>
-      <c r="P34">
-        <f>(1+O34)^92</f>
+      <c r="Q34">
+        <f t="shared" si="11"/>
         <v>1.22971499588866</v>
       </c>
     </row>
-    <row r="35" spans="2:16">
+    <row r="35" spans="2:17">
       <c r="B35" s="1">
         <v>44724</v>
       </c>
@@ -6442,47 +6541,50 @@
       <c r="E35">
         <v>20</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="19" cm="1">
+        <f t="array" ref="F35">SUMPRODUCT(($C$11:$C$51=C35)*($E$11:$E$51))</f>
+        <v>20</v>
+      </c>
+      <c r="G35">
         <v>47.95</v>
       </c>
-      <c r="G35">
+      <c r="H35">
+        <f t="shared" si="7"/>
+        <v>959</v>
+      </c>
+      <c r="I35" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="8"/>
+        <v>-959</v>
+      </c>
+      <c r="K35" t="s">
+        <v>415</v>
+      </c>
+      <c r="L35" t="s">
+        <v>163</v>
+      </c>
+      <c r="M35" s="1">
+        <v>44815</v>
+      </c>
+      <c r="N35">
+        <v>0.12</v>
+      </c>
+      <c r="O35">
         <f t="shared" si="9"/>
-        <v>959</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I35">
+        <v>91</v>
+      </c>
+      <c r="P35">
         <f t="shared" si="10"/>
-        <v>-959</v>
-      </c>
-      <c r="J35" t="s">
-        <v>415</v>
-      </c>
-      <c r="K35" t="s">
-        <v>163</v>
-      </c>
-      <c r="L35" s="1">
-        <v>44815</v>
-      </c>
-      <c r="M35">
-        <v>0.12</v>
-      </c>
-      <c r="N35">
-        <f>L35-B35</f>
-        <v>91</v>
-      </c>
-      <c r="O35">
-        <f>(1+M35)^(1/N35)-1</f>
         <v>1.2461459636541328E-3</v>
       </c>
-      <c r="P35">
-        <f>(1+O35)^92</f>
+      <c r="Q35">
+        <f t="shared" si="11"/>
         <v>1.1213956834792898</v>
       </c>
     </row>
-    <row r="36" spans="2:16">
+    <row r="36" spans="2:17">
       <c r="B36" s="1">
         <v>44724</v>
       </c>
@@ -6495,47 +6597,50 @@
       <c r="E36">
         <v>10</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="19" cm="1">
+        <f t="array" ref="F36">SUMPRODUCT(($C$11:$C$51=C36)*($E$11:$E$51))</f>
+        <v>10</v>
+      </c>
+      <c r="G36">
         <v>100.4</v>
       </c>
-      <c r="G36">
+      <c r="H36">
+        <f t="shared" si="7"/>
+        <v>1004</v>
+      </c>
+      <c r="I36" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="8"/>
+        <v>-1004</v>
+      </c>
+      <c r="K36" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="L36" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M36" s="1">
+        <v>44815</v>
+      </c>
+      <c r="N36">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O36" s="18">
         <f t="shared" si="9"/>
-        <v>1004</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I36">
+        <v>91</v>
+      </c>
+      <c r="P36" s="18">
         <f t="shared" si="10"/>
-        <v>-1004</v>
-      </c>
-      <c r="J36" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="K36" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="L36" s="1">
-        <v>44815</v>
-      </c>
-      <c r="M36">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="N36" s="18">
-        <f>L36-B36</f>
-        <v>91</v>
-      </c>
-      <c r="O36" s="18">
-        <f>(1+M36)^(1/N36)-1</f>
         <v>1.4409081274349145E-3</v>
       </c>
-      <c r="P36" s="18">
-        <f>(1+O36)^92</f>
+      <c r="Q36" s="18">
+        <f t="shared" si="11"/>
         <v>1.1416426352652658</v>
       </c>
     </row>
-    <row r="37" spans="2:16">
+    <row r="37" spans="2:17">
       <c r="B37" s="1">
         <v>44724</v>
       </c>
@@ -6548,47 +6653,50 @@
       <c r="E37">
         <v>14</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="19" cm="1">
+        <f t="array" ref="F37">SUMPRODUCT(($C$11:$C$51=C37)*($E$11:$E$51))</f>
+        <v>14</v>
+      </c>
+      <c r="G37">
         <v>73.89</v>
       </c>
-      <c r="G37">
+      <c r="H37">
+        <f t="shared" si="7"/>
+        <v>1034.46</v>
+      </c>
+      <c r="I37" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="8"/>
+        <v>-1034.46</v>
+      </c>
+      <c r="K37" t="s">
+        <v>415</v>
+      </c>
+      <c r="L37" t="s">
+        <v>141</v>
+      </c>
+      <c r="M37" s="1">
+        <v>44815</v>
+      </c>
+      <c r="N37">
+        <v>0.35</v>
+      </c>
+      <c r="O37" s="18">
         <f t="shared" si="9"/>
-        <v>1034.46</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I37">
+        <v>91</v>
+      </c>
+      <c r="P37" s="18">
         <f t="shared" si="10"/>
-        <v>-1034.46</v>
-      </c>
-      <c r="J37" t="s">
-        <v>415</v>
-      </c>
-      <c r="K37" t="s">
-        <v>141</v>
-      </c>
-      <c r="L37" s="1">
-        <v>44815</v>
-      </c>
-      <c r="M37">
-        <v>0.35</v>
-      </c>
-      <c r="N37" s="18">
-        <f>L37-B37</f>
-        <v>91</v>
-      </c>
-      <c r="O37" s="18">
-        <f>(1+M37)^(1/N37)-1</f>
         <v>3.303296563134106E-3</v>
       </c>
-      <c r="P37" s="18">
-        <f>(1+O37)^92</f>
+      <c r="Q37" s="18">
+        <f t="shared" si="11"/>
         <v>1.3544594503602096</v>
       </c>
     </row>
-    <row r="38" spans="2:16">
+    <row r="38" spans="2:17">
       <c r="B38" s="1">
         <v>44724</v>
       </c>
@@ -6601,47 +6709,50 @@
       <c r="E38">
         <v>33</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="19" cm="1">
+        <f t="array" ref="F38">SUMPRODUCT(($C$11:$C$51=C38)*($E$11:$E$51))</f>
+        <v>33</v>
+      </c>
+      <c r="G38">
         <v>30.21</v>
       </c>
-      <c r="G38">
+      <c r="H38">
+        <f t="shared" si="7"/>
+        <v>996.93000000000006</v>
+      </c>
+      <c r="I38" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="8"/>
+        <v>-996.93000000000006</v>
+      </c>
+      <c r="K38" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="L38" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M38" s="1">
+        <v>44815</v>
+      </c>
+      <c r="N38" s="18">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="O38" s="18">
         <f t="shared" si="9"/>
-        <v>996.93000000000006</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I38">
+        <v>91</v>
+      </c>
+      <c r="P38" s="18">
         <f t="shared" si="10"/>
-        <v>-996.93000000000006</v>
-      </c>
-      <c r="J38" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="K38" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="L38" s="1">
-        <v>44815</v>
-      </c>
-      <c r="M38" s="18">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="N38" s="18">
-        <f>L38-B38</f>
-        <v>91</v>
-      </c>
-      <c r="O38" s="18">
-        <f>(1+M38)^(1/N38)-1</f>
         <v>2.7164309397338382E-3</v>
       </c>
-      <c r="P38" s="18">
-        <f>(1+O38)^92</f>
+      <c r="Q38" s="18">
+        <f t="shared" si="11"/>
         <v>1.2834770316028687</v>
       </c>
     </row>
-    <row r="39" spans="2:16">
+    <row r="39" spans="2:17">
       <c r="B39" s="1">
         <v>44724</v>
       </c>
@@ -6654,47 +6765,50 @@
       <c r="E39">
         <v>21</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="19" cm="1">
+        <f t="array" ref="F39">SUMPRODUCT(($C$11:$C$51=C39)*($E$11:$E$51))</f>
+        <v>41</v>
+      </c>
+      <c r="G39">
         <v>48.75</v>
       </c>
-      <c r="G39">
+      <c r="H39">
+        <f t="shared" si="7"/>
+        <v>1023.75</v>
+      </c>
+      <c r="I39" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="8"/>
+        <v>-1023.75</v>
+      </c>
+      <c r="K39" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="L39" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M39" s="1">
+        <v>44745</v>
+      </c>
+      <c r="N39">
+        <v>0.11</v>
+      </c>
+      <c r="O39">
         <f t="shared" si="9"/>
-        <v>1023.75</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I39">
+        <v>21</v>
+      </c>
+      <c r="P39">
         <f t="shared" si="10"/>
-        <v>-1023.75</v>
-      </c>
-      <c r="J39" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="K39" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="L39" s="1">
-        <v>44745</v>
-      </c>
-      <c r="M39">
-        <v>0.11</v>
-      </c>
-      <c r="N39">
-        <f>L39-B39</f>
-        <v>21</v>
-      </c>
-      <c r="O39">
-        <f>(1+M39)^(1/N39)-1</f>
         <v>4.981893106467794E-3</v>
       </c>
-      <c r="P39">
-        <f>(1+O39)^92</f>
+      <c r="Q39">
+        <f t="shared" si="11"/>
         <v>1.5796388699807264</v>
       </c>
     </row>
-    <row r="40" spans="2:16">
+    <row r="40" spans="2:17">
       <c r="B40" s="1">
         <v>44724</v>
       </c>
@@ -6707,47 +6821,50 @@
       <c r="E40">
         <v>7</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="19" cm="1">
+        <f t="array" ref="F40">SUMPRODUCT(($C$11:$C$51=C40)*($E$11:$E$51))</f>
+        <v>7</v>
+      </c>
+      <c r="G40">
         <v>144</v>
       </c>
-      <c r="G40">
+      <c r="H40">
+        <f t="shared" si="7"/>
+        <v>1008</v>
+      </c>
+      <c r="I40" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="8"/>
+        <v>-1008</v>
+      </c>
+      <c r="K40" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="L40" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M40" s="1">
+        <v>44815</v>
+      </c>
+      <c r="N40" s="18">
+        <v>0.11</v>
+      </c>
+      <c r="O40" s="18">
         <f t="shared" si="9"/>
-        <v>1008</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I40">
+        <v>91</v>
+      </c>
+      <c r="P40" s="18">
         <f t="shared" si="10"/>
-        <v>-1008</v>
-      </c>
-      <c r="J40" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="K40" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="L40" s="1">
-        <v>44815</v>
-      </c>
-      <c r="M40" s="18">
-        <v>0.11</v>
-      </c>
-      <c r="N40" s="18">
-        <f>L40-B40</f>
-        <v>91</v>
-      </c>
-      <c r="O40" s="18">
-        <f>(1+M40)^(1/N40)-1</f>
         <v>1.1474711970971274E-3</v>
       </c>
-      <c r="P40" s="18">
-        <f>(1+O40)^92</f>
+      <c r="Q40" s="18">
+        <f t="shared" si="11"/>
         <v>1.111273693028771</v>
       </c>
     </row>
-    <row r="41" spans="2:16">
+    <row r="41" spans="2:17">
       <c r="B41" s="1">
         <v>44724</v>
       </c>
@@ -6760,47 +6877,50 @@
       <c r="E41">
         <v>8</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="19" cm="1">
+        <f t="array" ref="F41">SUMPRODUCT(($C$11:$C$51=C41)*($E$11:$E$51))</f>
+        <v>8</v>
+      </c>
+      <c r="G41">
         <v>127.72</v>
       </c>
-      <c r="G41">
+      <c r="H41">
+        <f t="shared" si="7"/>
+        <v>1021.76</v>
+      </c>
+      <c r="I41" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="8"/>
+        <v>-1021.76</v>
+      </c>
+      <c r="K41" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="L41" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M41" s="1">
+        <v>44815</v>
+      </c>
+      <c r="N41">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="O41" s="18">
         <f t="shared" si="9"/>
-        <v>1021.76</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I41">
+        <v>91</v>
+      </c>
+      <c r="P41" s="18">
         <f t="shared" si="10"/>
-        <v>-1021.76</v>
-      </c>
-      <c r="J41" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="K41" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="L41" s="1">
-        <v>44815</v>
-      </c>
-      <c r="M41">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="N41" s="18">
-        <f>L41-B41</f>
-        <v>91</v>
-      </c>
-      <c r="O41" s="18">
-        <f>(1+M41)^(1/N41)-1</f>
         <v>1.0078392710637374E-3</v>
       </c>
-      <c r="P41" s="18">
-        <f>(1+O41)^92</f>
+      <c r="Q41" s="18">
+        <f t="shared" si="11"/>
         <v>1.0971045918410911</v>
       </c>
     </row>
-    <row r="42" spans="2:16">
+    <row r="42" spans="2:17">
       <c r="B42" s="1">
         <v>44724</v>
       </c>
@@ -6813,47 +6933,50 @@
       <c r="E42">
         <v>20</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="19" cm="1">
+        <f t="array" ref="F42">SUMPRODUCT(($C$11:$C$51=C42)*($E$11:$E$51))</f>
+        <v>20</v>
+      </c>
+      <c r="G42">
         <v>53.54</v>
       </c>
-      <c r="G42">
+      <c r="H42">
+        <f t="shared" si="7"/>
+        <v>1070.8</v>
+      </c>
+      <c r="I42" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="8"/>
+        <v>-1070.8</v>
+      </c>
+      <c r="K42" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="L42" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M42" s="1">
+        <v>44815</v>
+      </c>
+      <c r="N42">
+        <v>0.22</v>
+      </c>
+      <c r="O42" s="18">
         <f t="shared" si="9"/>
-        <v>1070.8</v>
-      </c>
-      <c r="H42">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I42">
+        <v>91</v>
+      </c>
+      <c r="P42" s="18">
         <f t="shared" si="10"/>
-        <v>-1070.8</v>
-      </c>
-      <c r="J42" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="K42" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="L42" s="1">
-        <v>44815</v>
-      </c>
-      <c r="M42">
-        <v>0.22</v>
-      </c>
-      <c r="N42" s="18">
-        <f>L42-B42</f>
-        <v>91</v>
-      </c>
-      <c r="O42" s="18">
-        <f>(1+M42)^(1/N42)-1</f>
         <v>2.1875635052042153E-3</v>
       </c>
-      <c r="P42" s="18">
-        <f>(1+O42)^92</f>
+      <c r="Q42" s="18">
+        <f t="shared" si="11"/>
         <v>1.222668827476334</v>
       </c>
     </row>
-    <row r="43" spans="2:16">
+    <row r="43" spans="2:17">
       <c r="B43" s="1">
         <v>44724</v>
       </c>
@@ -6866,47 +6989,50 @@
       <c r="E43">
         <v>20</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="19" cm="1">
+        <f t="array" ref="F43">SUMPRODUCT(($C$11:$C$51=C43)*($E$11:$E$51))</f>
+        <v>20</v>
+      </c>
+      <c r="G43">
         <v>51.5</v>
       </c>
-      <c r="G43">
+      <c r="H43">
+        <f t="shared" si="7"/>
+        <v>1030</v>
+      </c>
+      <c r="I43" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="8"/>
+        <v>-1030</v>
+      </c>
+      <c r="K43" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="L43" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M43" s="1">
+        <v>44815</v>
+      </c>
+      <c r="N43">
+        <v>0.73</v>
+      </c>
+      <c r="O43" s="18">
         <f t="shared" si="9"/>
-        <v>1030</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="I43">
+        <v>91</v>
+      </c>
+      <c r="P43" s="18">
         <f t="shared" si="10"/>
-        <v>-1030</v>
-      </c>
-      <c r="J43" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="K43" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="L43" s="1">
-        <v>44815</v>
-      </c>
-      <c r="M43">
-        <v>0.73</v>
-      </c>
-      <c r="N43" s="18">
-        <f>L43-B43</f>
-        <v>91</v>
-      </c>
-      <c r="O43" s="18">
-        <f>(1+M43)^(1/N43)-1</f>
         <v>6.0414888024045155E-3</v>
       </c>
-      <c r="P43" s="18">
-        <f>(1+O43)^92</f>
+      <c r="Q43" s="18">
+        <f t="shared" si="11"/>
         <v>1.7404517756281392</v>
       </c>
     </row>
-    <row r="44" spans="2:16">
+    <row r="44" spans="2:17">
       <c r="B44" s="1">
         <v>44724</v>
       </c>
@@ -6919,47 +7045,50 @@
       <c r="E44">
         <v>30</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="19" cm="1">
+        <f t="array" ref="F44">SUMPRODUCT(($C$11:$C$51=C44)*($E$11:$E$51))</f>
+        <v>30</v>
+      </c>
+      <c r="G44">
         <v>34.44</v>
       </c>
-      <c r="G44">
+      <c r="H44">
+        <f t="shared" si="7"/>
+        <v>1033.1999999999998</v>
+      </c>
+      <c r="I44" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J44" s="18">
+        <f t="shared" ref="J44:J45" si="12">I44*H44</f>
+        <v>-1033.1999999999998</v>
+      </c>
+      <c r="K44" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="L44" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M44" s="1">
+        <v>44815</v>
+      </c>
+      <c r="N44" s="18">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="O44" s="18">
         <f t="shared" si="9"/>
-        <v>1033.1999999999998</v>
-      </c>
-      <c r="H44" s="18">
-        <f t="shared" ref="H44:H45" si="11">IF(D44="Buy",-1,1)</f>
-        <v>-1</v>
-      </c>
-      <c r="I44" s="18">
-        <f t="shared" ref="I44:I45" si="12">H44*G44</f>
-        <v>-1033.1999999999998</v>
-      </c>
-      <c r="J44" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="K44" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="L44" s="1">
-        <v>44815</v>
-      </c>
-      <c r="M44" s="18">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="N44" s="18">
-        <f>L44-B44</f>
         <v>91</v>
       </c>
-      <c r="O44" s="18">
-        <f>(1+M44)^(1/N44)-1</f>
+      <c r="P44" s="18">
+        <f t="shared" si="10"/>
         <v>2.5865494959438351E-3</v>
       </c>
-      <c r="P44" s="18">
-        <f>(1+O44)^92</f>
+      <c r="Q44" s="18">
+        <f t="shared" si="11"/>
         <v>1.2682719851123665</v>
       </c>
     </row>
-    <row r="45" spans="2:16">
+    <row r="45" spans="2:17">
       <c r="B45" s="1">
         <v>44724</v>
       </c>
@@ -6972,47 +7101,50 @@
       <c r="E45">
         <v>23</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="19" cm="1">
+        <f t="array" ref="F45">SUMPRODUCT(($C$11:$C$51=C45)*($E$11:$E$51))</f>
+        <v>23</v>
+      </c>
+      <c r="G45">
         <v>44.15</v>
       </c>
-      <c r="G45">
-        <f t="shared" si="9"/>
+      <c r="H45">
+        <f t="shared" si="7"/>
         <v>1015.4499999999999</v>
       </c>
-      <c r="H45">
-        <f t="shared" si="11"/>
+      <c r="I45" s="19">
         <v>-1</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <f t="shared" si="12"/>
         <v>-1015.4499999999999</v>
       </c>
-      <c r="J45" s="18" t="s">
+      <c r="K45" s="18" t="s">
         <v>415</v>
       </c>
-      <c r="K45" s="18" t="s">
+      <c r="L45" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="L45" s="1">
+      <c r="M45" s="1">
         <v>44815</v>
       </c>
-      <c r="M45">
+      <c r="N45">
         <v>0.13</v>
       </c>
-      <c r="N45" s="18">
-        <f>L45-B45</f>
+      <c r="O45" s="18">
+        <f t="shared" si="9"/>
         <v>91</v>
       </c>
-      <c r="O45" s="18">
-        <f>(1+M45)^(1/N45)-1</f>
+      <c r="P45" s="18">
+        <f t="shared" si="10"/>
         <v>1.3439532058281412E-3</v>
       </c>
-      <c r="P45" s="18">
-        <f>(1+O45)^92</f>
+      <c r="Q45" s="18">
+        <f t="shared" si="11"/>
         <v>1.1315186671225852</v>
       </c>
     </row>
-    <row r="46" spans="2:16">
+    <row r="46" spans="2:17">
       <c r="B46" s="1">
         <v>44724</v>
       </c>
@@ -7025,47 +7157,50 @@
       <c r="E46">
         <v>15</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="19" cm="1">
+        <f t="array" ref="F46">SUMPRODUCT(($C$11:$C$51=C46)*($E$11:$E$51))</f>
+        <v>15</v>
+      </c>
+      <c r="G46">
         <v>66.5</v>
       </c>
-      <c r="G46">
+      <c r="H46">
+        <f t="shared" si="7"/>
+        <v>997.5</v>
+      </c>
+      <c r="I46" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J46" s="18">
+        <f t="shared" ref="J46" si="13">I46*H46</f>
+        <v>-997.5</v>
+      </c>
+      <c r="K46" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="L46" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M46" s="1">
+        <v>44815</v>
+      </c>
+      <c r="N46">
+        <v>0.16</v>
+      </c>
+      <c r="O46" s="18">
         <f t="shared" si="9"/>
-        <v>997.5</v>
-      </c>
-      <c r="H46" s="18">
-        <f t="shared" ref="H46" si="13">IF(D46="Buy",-1,1)</f>
-        <v>-1</v>
-      </c>
-      <c r="I46" s="18">
-        <f t="shared" ref="I46" si="14">H46*G46</f>
-        <v>-997.5</v>
-      </c>
-      <c r="J46" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="K46" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="L46" s="1">
-        <v>44815</v>
-      </c>
-      <c r="M46">
-        <v>0.16</v>
-      </c>
-      <c r="N46" s="18">
-        <f>L46-B46</f>
         <v>91</v>
       </c>
-      <c r="O46" s="18">
-        <f>(1+M46)^(1/N46)-1</f>
+      <c r="P46" s="18">
+        <f t="shared" si="10"/>
         <v>1.6323198533032546E-3</v>
       </c>
-      <c r="P46" s="18">
-        <f>(1+O46)^92</f>
+      <c r="Q46" s="18">
+        <f t="shared" si="11"/>
         <v>1.1618934910298244</v>
       </c>
     </row>
-    <row r="47" spans="2:16">
+    <row r="47" spans="2:17">
       <c r="B47" s="1">
         <v>44724</v>
       </c>
@@ -7078,47 +7213,50 @@
       <c r="E47">
         <v>4</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="19" cm="1">
+        <f t="array" ref="F47">SUMPRODUCT(($C$11:$C$51=C47)*($E$11:$E$51))</f>
+        <v>4</v>
+      </c>
+      <c r="G47">
         <v>270.8</v>
       </c>
-      <c r="G47">
+      <c r="H47">
+        <f t="shared" si="7"/>
+        <v>1083.2</v>
+      </c>
+      <c r="I47" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J47" s="18">
+        <f t="shared" ref="J47" si="14">I47*H47</f>
+        <v>-1083.2</v>
+      </c>
+      <c r="K47" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="L47" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M47" s="1">
+        <v>44815</v>
+      </c>
+      <c r="N47" s="18">
+        <v>0.09</v>
+      </c>
+      <c r="O47" s="18">
         <f t="shared" si="9"/>
-        <v>1083.2</v>
-      </c>
-      <c r="H47" s="18">
-        <f t="shared" ref="H47" si="15">IF(D47="Buy",-1,1)</f>
-        <v>-1</v>
-      </c>
-      <c r="I47" s="18">
-        <f t="shared" ref="I47" si="16">H47*G47</f>
-        <v>-1083.2</v>
-      </c>
-      <c r="J47" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="K47" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="L47" s="1">
-        <v>44815</v>
-      </c>
-      <c r="M47" s="18">
-        <v>0.09</v>
-      </c>
-      <c r="N47" s="18">
-        <f>L47-B47</f>
         <v>91</v>
       </c>
-      <c r="O47" s="18">
-        <f>(1+M47)^(1/N47)-1</f>
+      <c r="P47" s="18">
+        <f t="shared" si="10"/>
         <v>9.4745620432945543E-4</v>
       </c>
-      <c r="P47" s="18">
-        <f>(1+O47)^92</f>
+      <c r="Q47" s="18">
+        <f t="shared" si="11"/>
         <v>1.0910327272627209</v>
       </c>
     </row>
-    <row r="48" spans="2:16">
+    <row r="48" spans="2:17">
       <c r="B48" s="1">
         <v>44724</v>
       </c>
@@ -7131,47 +7269,50 @@
       <c r="E48">
         <v>16</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="19" cm="1">
+        <f t="array" ref="F48">SUMPRODUCT(($C$11:$C$51=C48)*($E$11:$E$51))</f>
+        <v>16</v>
+      </c>
+      <c r="G48">
         <v>63.54</v>
       </c>
-      <c r="G48">
+      <c r="H48">
+        <f t="shared" si="7"/>
+        <v>1016.64</v>
+      </c>
+      <c r="I48" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J48" s="18">
+        <f t="shared" ref="J48" si="15">I48*H48</f>
+        <v>-1016.64</v>
+      </c>
+      <c r="K48" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="L48" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M48" s="1">
+        <v>44815</v>
+      </c>
+      <c r="N48" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="O48" s="18">
         <f t="shared" si="9"/>
-        <v>1016.64</v>
-      </c>
-      <c r="H48" s="18">
-        <f t="shared" ref="H48" si="17">IF(D48="Buy",-1,1)</f>
-        <v>-1</v>
-      </c>
-      <c r="I48" s="18">
-        <f t="shared" ref="I48" si="18">H48*G48</f>
-        <v>-1016.64</v>
-      </c>
-      <c r="J48" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="K48" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="L48" s="1">
-        <v>44815</v>
-      </c>
-      <c r="M48" s="18">
-        <v>0.3</v>
-      </c>
-      <c r="N48" s="18">
-        <f>L48-B48</f>
         <v>91</v>
       </c>
-      <c r="O48" s="18">
-        <f>(1+M48)^(1/N48)-1</f>
+      <c r="P48" s="18">
+        <f t="shared" si="10"/>
         <v>2.8872839838995912E-3</v>
       </c>
-      <c r="P48" s="18">
-        <f>(1+O48)^92</f>
+      <c r="Q48" s="18">
+        <f t="shared" si="11"/>
         <v>1.3037534691790746</v>
       </c>
     </row>
-    <row r="49" spans="2:16">
+    <row r="49" spans="2:17">
       <c r="B49" s="1">
         <v>44724</v>
       </c>
@@ -7184,47 +7325,50 @@
       <c r="E49">
         <v>12</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="19" cm="1">
+        <f t="array" ref="F49">SUMPRODUCT(($C$11:$C$51=C49)*($E$11:$E$51))</f>
+        <v>12</v>
+      </c>
+      <c r="G49">
         <v>86.3</v>
       </c>
-      <c r="G49">
+      <c r="H49">
+        <f t="shared" si="7"/>
+        <v>1035.5999999999999</v>
+      </c>
+      <c r="I49" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J49" s="18">
+        <f t="shared" ref="J49:J50" si="16">I49*H49</f>
+        <v>-1035.5999999999999</v>
+      </c>
+      <c r="K49" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="L49" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="M49" s="1">
+        <v>44801</v>
+      </c>
+      <c r="N49">
+        <v>0.12</v>
+      </c>
+      <c r="O49" s="18">
         <f t="shared" si="9"/>
-        <v>1035.5999999999999</v>
-      </c>
-      <c r="H49" s="18">
-        <f t="shared" ref="H49:H50" si="19">IF(D49="Buy",-1,1)</f>
-        <v>-1</v>
-      </c>
-      <c r="I49" s="18">
-        <f t="shared" ref="I49:I50" si="20">H49*G49</f>
-        <v>-1035.5999999999999</v>
-      </c>
-      <c r="J49" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="K49" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="L49" s="1">
-        <v>44801</v>
-      </c>
-      <c r="M49">
-        <v>0.12</v>
-      </c>
-      <c r="N49" s="18">
-        <f>L49-B49</f>
         <v>77</v>
       </c>
-      <c r="O49" s="18">
-        <f>(1+M49)^(1/N49)-1</f>
+      <c r="P49" s="18">
+        <f t="shared" si="10"/>
         <v>1.4728847386982213E-3</v>
       </c>
-      <c r="P49" s="18">
-        <f>(1+O49)^92</f>
+      <c r="Q49" s="18">
+        <f t="shared" si="11"/>
         <v>1.1450012193329568</v>
       </c>
     </row>
-    <row r="50" spans="2:16">
+    <row r="50" spans="2:17">
       <c r="B50" s="1">
         <v>44724</v>
       </c>
@@ -7237,47 +7381,50 @@
       <c r="E50">
         <v>13</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="19" cm="1">
+        <f t="array" ref="F50">SUMPRODUCT(($C$11:$C$51=C50)*($E$11:$E$51))</f>
+        <v>13</v>
+      </c>
+      <c r="G50">
         <v>76.400000000000006</v>
       </c>
-      <c r="G50">
+      <c r="H50">
+        <f t="shared" si="7"/>
+        <v>993.2</v>
+      </c>
+      <c r="I50" s="19">
+        <v>-1</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="16"/>
+        <v>-993.2</v>
+      </c>
+      <c r="K50" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="L50" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="M50" s="1">
+        <v>44780</v>
+      </c>
+      <c r="N50">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="O50" s="18">
         <f t="shared" si="9"/>
-        <v>993.2</v>
-      </c>
-      <c r="H50">
-        <f t="shared" si="19"/>
-        <v>-1</v>
-      </c>
-      <c r="I50">
-        <f t="shared" si="20"/>
-        <v>-993.2</v>
-      </c>
-      <c r="J50" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="K50" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="L50" s="1">
-        <v>44780</v>
-      </c>
-      <c r="M50">
-        <v>9.4899999999999998E-2</v>
-      </c>
-      <c r="N50" s="18">
-        <f>L50-B50</f>
         <v>56</v>
       </c>
-      <c r="O50" s="18">
-        <f>(1+M50)^(1/N50)-1</f>
+      <c r="P50" s="18">
+        <f t="shared" si="10"/>
         <v>1.6202940261609289E-3</v>
       </c>
-      <c r="P50" s="18">
-        <f>(1+O50)^92</f>
+      <c r="Q50" s="18">
+        <f t="shared" si="11"/>
         <v>1.1606107956028482</v>
       </c>
     </row>
-    <row r="51" spans="2:16">
+    <row r="51" spans="2:17">
       <c r="B51" s="1">
         <v>44724</v>
       </c>
@@ -7290,48 +7437,51 @@
       <c r="E51" s="18">
         <v>7</v>
       </c>
-      <c r="F51" s="18">
+      <c r="F51" s="19" cm="1">
+        <f t="array" ref="F51">SUMPRODUCT(($C$11:$C$51=C51)*($E$11:$E$51))</f>
+        <v>7</v>
+      </c>
+      <c r="G51" s="18">
         <v>155.49</v>
       </c>
-      <c r="G51" s="18">
-        <f t="shared" ref="G51" si="21">F51*E51</f>
+      <c r="H51" s="18">
+        <f t="shared" ref="H51" si="17">G51*E51</f>
         <v>1088.43</v>
       </c>
-      <c r="H51" s="18">
-        <f t="shared" ref="H51" si="22">IF(D51="Buy",-1,1)</f>
+      <c r="I51" s="19">
         <v>-1</v>
       </c>
-      <c r="I51" s="18">
-        <f t="shared" ref="I51" si="23">H51*G51</f>
+      <c r="J51" s="18">
+        <f t="shared" ref="J51" si="18">I51*H51</f>
         <v>-1088.43</v>
       </c>
-      <c r="J51" s="18" t="s">
+      <c r="K51" s="18" t="s">
         <v>415</v>
       </c>
-      <c r="K51" s="18" t="s">
+      <c r="L51" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="L51" s="1">
+      <c r="M51" s="1">
         <v>44815</v>
       </c>
-      <c r="M51">
+      <c r="N51">
         <v>0.14000000000000001</v>
       </c>
-      <c r="N51" s="18">
-        <f>L51-B51</f>
+      <c r="O51" s="18">
+        <f t="shared" si="9"/>
         <v>91</v>
       </c>
-      <c r="O51" s="18">
-        <f>(1+M51)^(1/N51)-1</f>
+      <c r="P51" s="18">
+        <f t="shared" si="10"/>
         <v>1.4409081274349145E-3</v>
       </c>
-      <c r="P51" s="18">
-        <f>(1+O51)^92</f>
+      <c r="Q51" s="18">
+        <f t="shared" si="11"/>
         <v>1.1416426352652658</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O26:O51">
+  <conditionalFormatting sqref="P26:P51">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -7604,10 +7754,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="20"/>
+      <c r="B38" s="28"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="6"/>
@@ -7664,10 +7814,10 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="20"/>
+      <c r="B47" s="28"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="6"/>
@@ -7990,10 +8140,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="20"/>
+      <c r="B35" s="28"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -8050,10 +8200,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="20"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -8550,10 +8700,10 @@
       <c r="A14" s="10"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="20"/>
+      <c r="B15" s="28"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6"/>
@@ -8610,10 +8760,10 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="20"/>
+      <c r="B24" s="28"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6"/>
@@ -8928,10 +9078,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="20"/>
+      <c r="B32" s="28"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -8988,10 +9138,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="20"/>
+      <c r="B41" s="28"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -9515,10 +9665,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="20"/>
+      <c r="B35" s="28"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -9575,10 +9725,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="20"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -9906,10 +10056,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="20"/>
+      <c r="B35" s="28"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -9966,10 +10116,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="20"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -11109,10 +11259,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="20"/>
+      <c r="B35" s="28"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -11169,10 +11319,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="20"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -11785,10 +11935,10 @@
       <c r="A62" s="10"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="19" t="s">
+      <c r="A63" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="20"/>
+      <c r="B63" s="28"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6"/>
@@ -11845,10 +11995,10 @@
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="B72" s="20"/>
+      <c r="B72" s="28"/>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="6"/>
@@ -12308,10 +12458,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="20"/>
+      <c r="B32" s="28"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -12368,10 +12518,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="20"/>
+      <c r="B41" s="28"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -13240,37 +13390,37 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="20" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>497</v>
       </c>
     </row>
@@ -13278,12 +13428,12 @@
       <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="20" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>498</v>
       </c>
     </row>
@@ -13291,12 +13441,12 @@
       <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="20" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="20" t="s">
         <v>500</v>
       </c>
     </row>
@@ -13304,12 +13454,12 @@
       <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="20" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="20" t="s">
         <v>502</v>
       </c>
     </row>
@@ -13317,12 +13467,12 @@
       <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="20" t="s">
         <v>503</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="20" t="s">
         <v>504</v>
       </c>
     </row>
@@ -13330,12 +13480,12 @@
       <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="20" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="20" t="s">
         <v>506</v>
       </c>
     </row>
@@ -13343,12 +13493,12 @@
       <c r="A23" s="2"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="20" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="20" t="s">
         <v>508</v>
       </c>
     </row>
@@ -13409,7 +13559,7 @@
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="23"/>
+      <c r="A28" s="22"/>
     </row>
     <row r="29" spans="1:9" ht="30">
       <c r="A29" s="12"/>
@@ -13456,13 +13606,13 @@
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="23"/>
+      <c r="A31" s="22"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="20"/>
+      <c r="B32" s="28"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="12"/>
@@ -13511,18 +13661,18 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="22"/>
+      <c r="A39" s="21"/>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="22" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="20"/>
+      <c r="B41" s="28"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="12"/>
@@ -13547,168 +13697,168 @@
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="25"/>
+      <c r="A46" s="23"/>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="20" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="20" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="21" t="s">
+      <c r="A49" s="20" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="21" t="s">
+      <c r="A50" s="20" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="21" t="s">
+      <c r="A51" s="20" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="21" t="s">
+      <c r="A52" s="20" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="20" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="25"/>
+      <c r="A54" s="23"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="20" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="20" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="21" t="s">
+      <c r="A57" s="20" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="21" t="s">
+      <c r="A58" s="20" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="21" t="s">
+      <c r="A59" s="20" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="21" t="s">
+      <c r="A60" s="20" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="21" t="s">
+      <c r="A61" s="20" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="21" t="s">
+      <c r="A62" s="20" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="21" t="s">
+      <c r="A63" s="20" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="21" t="s">
+      <c r="A64" s="20" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="21" t="s">
+      <c r="A65" s="20" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="21" t="s">
+      <c r="A66" s="20" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="21" t="s">
+      <c r="A67" s="20" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="21" t="s">
+      <c r="A68" s="20" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="21" t="s">
+      <c r="A69" s="20" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="21" t="s">
+      <c r="A70" s="20" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="21" t="s">
+      <c r="A71" s="20" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="21" t="s">
+      <c r="A72" s="20" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="21" t="s">
+      <c r="A73" s="20" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="21" t="s">
+      <c r="A74" s="20" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="21" t="s">
+      <c r="A75" s="20" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="21" t="s">
+      <c r="A76" s="20" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="21" t="s">
+      <c r="A77" s="20" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="21" t="s">
+      <c r="A78" s="20" t="s">
         <v>535</v>
       </c>
     </row>
@@ -13716,207 +13866,207 @@
       <c r="A79" s="2"/>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="21" t="s">
+      <c r="A80" s="20" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="21" t="s">
+      <c r="A81" s="20" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="21" t="s">
+      <c r="A82" s="20" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="21" t="s">
+      <c r="A83" s="20" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="21" t="s">
+      <c r="A84" s="20" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="21" t="s">
+      <c r="A85" s="20" t="s">
         <v>540</v>
       </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="21" t="s">
+      <c r="A86" s="20" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="21" t="s">
+      <c r="A87" s="20" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="21" t="s">
+      <c r="A88" s="20" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="21" t="s">
+      <c r="A89" s="20" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="21" t="s">
+      <c r="A90" s="20" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="21" t="s">
+      <c r="A91" s="20" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="21" t="s">
+      <c r="A92" s="20" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="21" t="s">
+      <c r="A93" s="20" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="21" t="s">
+      <c r="A94" s="20" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="21" t="s">
+      <c r="A95" s="20" t="s">
         <v>550</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="21" t="s">
+      <c r="A96" s="20" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="21" t="s">
+      <c r="A97" s="20" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="21" t="s">
+      <c r="A98" s="20" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="21" t="s">
+      <c r="A99" s="20" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="21" t="s">
+      <c r="A100" s="20" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="21" t="s">
+      <c r="A101" s="20" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="21" t="s">
+      <c r="A102" s="20" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="21" t="s">
+      <c r="A103" s="20" t="s">
         <v>558</v>
       </c>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="21" t="s">
+      <c r="A104" s="20" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="21" t="s">
+      <c r="A105" s="20" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="21" t="s">
+      <c r="A106" s="20" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="21" t="s">
+      <c r="A107" s="20" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="108" spans="1:1">
-      <c r="A108" s="21" t="s">
+      <c r="A108" s="20" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="109" spans="1:1">
-      <c r="A109" s="21" t="s">
+      <c r="A109" s="20" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="110" spans="1:1">
-      <c r="A110" s="21" t="s">
+      <c r="A110" s="20" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="111" spans="1:1">
-      <c r="A111" s="21" t="s">
+      <c r="A111" s="20" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="112" spans="1:1">
-      <c r="A112" s="21" t="s">
+      <c r="A112" s="20" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="113" spans="1:1">
-      <c r="A113" s="21" t="s">
+      <c r="A113" s="20" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="114" spans="1:1">
-      <c r="A114" s="21" t="s">
+      <c r="A114" s="20" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="115" spans="1:1">
-      <c r="A115" s="21" t="s">
+      <c r="A115" s="20" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="116" spans="1:1">
-      <c r="A116" s="21" t="s">
+      <c r="A116" s="20" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="117" spans="1:1">
-      <c r="A117" s="21" t="s">
+      <c r="A117" s="20" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="118" spans="1:1">
-      <c r="A118" s="21" t="s">
+      <c r="A118" s="20" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="119" spans="1:1">
-      <c r="A119" s="21" t="s">
+      <c r="A119" s="20" t="s">
         <v>574</v>
       </c>
     </row>
     <row r="120" spans="1:1">
-      <c r="A120" s="21" t="s">
+      <c r="A120" s="20" t="s">
         <v>575</v>
       </c>
     </row>
@@ -13924,232 +14074,232 @@
       <c r="A121" s="2"/>
     </row>
     <row r="122" spans="1:1">
-      <c r="A122" s="21" t="s">
+      <c r="A122" s="20" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="123" spans="1:1">
-      <c r="A123" s="21" t="s">
+      <c r="A123" s="20" t="s">
         <v>577</v>
       </c>
     </row>
     <row r="124" spans="1:1">
-      <c r="A124" s="21" t="s">
+      <c r="A124" s="20" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="125" spans="1:1">
-      <c r="A125" s="21" t="s">
+      <c r="A125" s="20" t="s">
         <v>579</v>
       </c>
     </row>
     <row r="126" spans="1:1">
-      <c r="A126" s="21" t="s">
+      <c r="A126" s="20" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="127" spans="1:1">
-      <c r="A127" s="21" t="s">
+      <c r="A127" s="20" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="128" spans="1:1">
-      <c r="A128" s="21" t="s">
+      <c r="A128" s="20" t="s">
         <v>582</v>
       </c>
     </row>
     <row r="129" spans="1:1">
-      <c r="A129" s="21" t="s">
+      <c r="A129" s="20" t="s">
         <v>583</v>
       </c>
     </row>
     <row r="130" spans="1:1">
-      <c r="A130" s="21" t="s">
+      <c r="A130" s="20" t="s">
         <v>584</v>
       </c>
     </row>
     <row r="131" spans="1:1">
-      <c r="A131" s="21" t="s">
+      <c r="A131" s="20" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="21" t="s">
+      <c r="A132" s="20" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="133" spans="1:1">
-      <c r="A133" s="21" t="s">
+      <c r="A133" s="20" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="21" t="s">
+      <c r="A134" s="20" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="135" spans="1:1">
-      <c r="A135" s="21" t="s">
+      <c r="A135" s="20" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="136" spans="1:1">
-      <c r="A136" s="21" t="s">
+      <c r="A136" s="20" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="137" spans="1:1">
-      <c r="A137" s="21" t="s">
+      <c r="A137" s="20" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="138" spans="1:1">
-      <c r="A138" s="21" t="s">
+      <c r="A138" s="20" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="139" spans="1:1">
-      <c r="A139" s="21" t="s">
+      <c r="A139" s="20" t="s">
         <v>593</v>
       </c>
     </row>
     <row r="140" spans="1:1">
-      <c r="A140" s="21" t="s">
+      <c r="A140" s="20" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="141" spans="1:1">
-      <c r="A141" s="21" t="s">
+      <c r="A141" s="20" t="s">
         <v>595</v>
       </c>
     </row>
     <row r="142" spans="1:1">
-      <c r="A142" s="21" t="s">
+      <c r="A142" s="20" t="s">
         <v>596</v>
       </c>
     </row>
     <row r="143" spans="1:1">
-      <c r="A143" s="21" t="s">
+      <c r="A143" s="20" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="144" spans="1:1">
-      <c r="A144" s="21" t="s">
+      <c r="A144" s="20" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="145" spans="1:1">
-      <c r="A145" s="21" t="s">
+      <c r="A145" s="20" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="146" spans="1:1">
-      <c r="A146" s="21" t="s">
+      <c r="A146" s="20" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="147" spans="1:1">
-      <c r="A147" s="21" t="s">
+      <c r="A147" s="20" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="148" spans="1:1">
-      <c r="A148" s="21" t="s">
+      <c r="A148" s="20" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="149" spans="1:1">
-      <c r="A149" s="21" t="s">
+      <c r="A149" s="20" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="150" spans="1:1">
-      <c r="A150" s="21" t="s">
+      <c r="A150" s="20" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="151" spans="1:1">
-      <c r="A151" s="21" t="s">
+      <c r="A151" s="20" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="152" spans="1:1">
-      <c r="A152" s="21" t="s">
+      <c r="A152" s="20" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="153" spans="1:1">
-      <c r="A153" s="21" t="s">
+      <c r="A153" s="20" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="154" spans="1:1">
-      <c r="A154" s="21" t="s">
+      <c r="A154" s="20" t="s">
         <v>608</v>
       </c>
     </row>
     <row r="155" spans="1:1">
-      <c r="A155" s="21" t="s">
+      <c r="A155" s="20" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="156" spans="1:1">
-      <c r="A156" s="21" t="s">
+      <c r="A156" s="20" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="157" spans="1:1">
-      <c r="A157" s="21" t="s">
+      <c r="A157" s="20" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="158" spans="1:1">
-      <c r="A158" s="21" t="s">
+      <c r="A158" s="20" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="159" spans="1:1">
-      <c r="A159" s="21" t="s">
+      <c r="A159" s="20" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="160" spans="1:1">
-      <c r="A160" s="21" t="s">
+      <c r="A160" s="20" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="161" spans="1:1">
-      <c r="A161" s="21" t="s">
+      <c r="A161" s="20" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="162" spans="1:1">
-      <c r="A162" s="21" t="s">
+      <c r="A162" s="20" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="163" spans="1:1">
-      <c r="A163" s="21" t="s">
+      <c r="A163" s="20" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="21" t="s">
+      <c r="A164" s="20" t="s">
         <v>618</v>
       </c>
     </row>
     <row r="165" spans="1:1">
-      <c r="A165" s="21" t="s">
+      <c r="A165" s="20" t="s">
         <v>619</v>
       </c>
     </row>
     <row r="166" spans="1:1">
-      <c r="A166" s="21" t="s">
+      <c r="A166" s="20" t="s">
         <v>620</v>
       </c>
     </row>
     <row r="167" spans="1:1">
-      <c r="A167" s="21" t="s">
+      <c r="A167" s="20" t="s">
         <v>621</v>
       </c>
     </row>
@@ -14157,172 +14307,172 @@
       <c r="A168" s="2"/>
     </row>
     <row r="169" spans="1:1">
-      <c r="A169" s="21" t="s">
+      <c r="A169" s="20" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="170" spans="1:1">
-      <c r="A170" s="21" t="s">
+      <c r="A170" s="20" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" s="21" t="s">
+      <c r="A171" s="20" t="s">
         <v>624</v>
       </c>
     </row>
     <row r="172" spans="1:1">
-      <c r="A172" s="21" t="s">
+      <c r="A172" s="20" t="s">
         <v>625</v>
       </c>
     </row>
     <row r="173" spans="1:1">
-      <c r="A173" s="21" t="s">
+      <c r="A173" s="20" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="174" spans="1:1">
-      <c r="A174" s="21" t="s">
+      <c r="A174" s="20" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="175" spans="1:1">
-      <c r="A175" s="21" t="s">
+      <c r="A175" s="20" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="176" spans="1:1">
-      <c r="A176" s="21" t="s">
+      <c r="A176" s="20" t="s">
         <v>629</v>
       </c>
     </row>
     <row r="177" spans="1:1">
-      <c r="A177" s="21" t="s">
+      <c r="A177" s="20" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="178" spans="1:1">
-      <c r="A178" s="21" t="s">
+      <c r="A178" s="20" t="s">
         <v>631</v>
       </c>
     </row>
     <row r="179" spans="1:1">
-      <c r="A179" s="21" t="s">
+      <c r="A179" s="20" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="180" spans="1:1">
-      <c r="A180" s="21" t="s">
+      <c r="A180" s="20" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="181" spans="1:1">
-      <c r="A181" s="21" t="s">
+      <c r="A181" s="20" t="s">
         <v>634</v>
       </c>
     </row>
     <row r="182" spans="1:1">
-      <c r="A182" s="21" t="s">
+      <c r="A182" s="20" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="183" spans="1:1">
-      <c r="A183" s="21" t="s">
+      <c r="A183" s="20" t="s">
         <v>636</v>
       </c>
     </row>
     <row r="184" spans="1:1">
-      <c r="A184" s="21" t="s">
+      <c r="A184" s="20" t="s">
         <v>637</v>
       </c>
     </row>
     <row r="185" spans="1:1">
-      <c r="A185" s="21" t="s">
+      <c r="A185" s="20" t="s">
         <v>638</v>
       </c>
     </row>
     <row r="186" spans="1:1">
-      <c r="A186" s="21" t="s">
+      <c r="A186" s="20" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="187" spans="1:1">
-      <c r="A187" s="21" t="s">
+      <c r="A187" s="20" t="s">
         <v>640</v>
       </c>
     </row>
     <row r="188" spans="1:1">
-      <c r="A188" s="21" t="s">
+      <c r="A188" s="20" t="s">
         <v>641</v>
       </c>
     </row>
     <row r="189" spans="1:1">
-      <c r="A189" s="21" t="s">
+      <c r="A189" s="20" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="190" spans="1:1">
-      <c r="A190" s="21" t="s">
+      <c r="A190" s="20" t="s">
         <v>643</v>
       </c>
     </row>
     <row r="191" spans="1:1">
-      <c r="A191" s="21" t="s">
+      <c r="A191" s="20" t="s">
         <v>644</v>
       </c>
     </row>
     <row r="192" spans="1:1">
-      <c r="A192" s="21" t="s">
+      <c r="A192" s="20" t="s">
         <v>645</v>
       </c>
     </row>
     <row r="193" spans="1:1">
-      <c r="A193" s="21" t="s">
+      <c r="A193" s="20" t="s">
         <v>646</v>
       </c>
     </row>
     <row r="194" spans="1:1">
-      <c r="A194" s="21" t="s">
+      <c r="A194" s="20" t="s">
         <v>647</v>
       </c>
     </row>
     <row r="195" spans="1:1">
-      <c r="A195" s="21" t="s">
+      <c r="A195" s="20" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="196" spans="1:1">
-      <c r="A196" s="21" t="s">
+      <c r="A196" s="20" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="197" spans="1:1">
-      <c r="A197" s="21" t="s">
+      <c r="A197" s="20" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="198" spans="1:1">
-      <c r="A198" s="21" t="s">
+      <c r="A198" s="20" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="199" spans="1:1">
-      <c r="A199" s="21" t="s">
+      <c r="A199" s="20" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="200" spans="1:1">
-      <c r="A200" s="21" t="s">
+      <c r="A200" s="20" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="201" spans="1:1">
-      <c r="A201" s="21" t="s">
+      <c r="A201" s="20" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" s="21" t="s">
+      <c r="A202" s="20" t="s">
         <v>655</v>
       </c>
     </row>
@@ -14330,75 +14480,75 @@
       <c r="A203" s="2"/>
     </row>
     <row r="204" spans="1:1">
-      <c r="A204" s="21" t="s">
+      <c r="A204" s="20" t="s">
         <v>656</v>
       </c>
     </row>
     <row r="205" spans="1:1">
-      <c r="A205" s="21" t="s">
+      <c r="A205" s="20" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="206" spans="1:1">
-      <c r="A206" s="21" t="s">
+      <c r="A206" s="20" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="207" spans="1:1">
-      <c r="A207" s="21" t="s">
+      <c r="A207" s="20" t="s">
         <v>659</v>
       </c>
     </row>
     <row r="208" spans="1:1">
-      <c r="A208" s="21" t="s">
+      <c r="A208" s="20" t="s">
         <v>660</v>
       </c>
     </row>
     <row r="209" spans="1:1">
-      <c r="A209" s="21" t="s">
+      <c r="A209" s="20" t="s">
         <v>661</v>
       </c>
     </row>
     <row r="210" spans="1:1">
-      <c r="A210" s="21" t="s">
+      <c r="A210" s="20" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="211" spans="1:1">
-      <c r="A211" s="21" t="s">
+      <c r="A211" s="20" t="s">
         <v>663</v>
       </c>
     </row>
     <row r="212" spans="1:1">
-      <c r="A212" s="21" t="s">
+      <c r="A212" s="20" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="213" spans="1:1">
-      <c r="A213" s="21" t="s">
+      <c r="A213" s="20" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="214" spans="1:1">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="20" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="215" spans="1:1">
-      <c r="A215" s="21" t="s">
+      <c r="A215" s="20" t="s">
         <v>667</v>
       </c>
     </row>
     <row r="216" spans="1:1">
-      <c r="A216" s="26" t="s">
+      <c r="A216" s="24" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="217" spans="1:1">
-      <c r="A217" s="27"/>
+      <c r="A217" s="25"/>
     </row>
     <row r="218" spans="1:1">
-      <c r="A218" s="28" t="s">
+      <c r="A218" s="26" t="s">
         <v>669</v>
       </c>
     </row>
@@ -14683,10 +14833,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="20"/>
+      <c r="B35" s="28"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -14743,10 +14893,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="20"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -15232,10 +15382,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="20"/>
+      <c r="B38" s="28"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6"/>
@@ -15292,10 +15442,10 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="20"/>
+      <c r="B47" s="28"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6"/>

</xml_diff>

<commit_message>
created a new business cycles notebook
</commit_message>
<xml_diff>
--- a/code/Screener/record.xlsx
+++ b/code/Screener/record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D51336-BEC4-49F3-B6ED-E05DD65B65C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CCBBB0-6A95-4BA7-A98E-8B93B69BC0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="1" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
   <sheets>
     <sheet name="Record book" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="1124">
   <si>
     <t>EXC</t>
   </si>
@@ -3441,6 +3441,9 @@
   </si>
   <si>
     <t>MGPI</t>
+  </si>
+  <si>
+    <t>Stop Loss</t>
   </si>
 </sst>
 </file>
@@ -3547,7 +3550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3621,6 +3624,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3669,7 +3674,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3730,7 +3735,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3796,7 +3801,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3857,7 +3862,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3923,7 +3928,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3984,7 +3989,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4045,7 +4050,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4111,7 +4116,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4172,7 +4177,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4238,7 +4243,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4299,7 +4304,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4346,133 +4351,6 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="9715500"/>
-          <a:ext cx="4819650" cy="3800475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="11258550"/>
-          <a:ext cx="4572000" cy="3676650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -4544,6 +4422,133 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="11258550"/>
+          <a:ext cx="4572000" cy="3676650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="9715500"/>
+          <a:ext cx="4819650" cy="3800475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -4553,7 +4558,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4619,7 +4624,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4680,7 +4685,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4746,7 +4751,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4807,7 +4812,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4873,7 +4878,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4934,7 +4939,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5000,7 +5005,7 @@
                   <a14:compatExt spid="_x0000_s10243"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003280000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000003280000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5050,7 +5055,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5111,7 +5116,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5177,7 +5182,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5238,7 +5243,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5304,7 +5309,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5365,7 +5370,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5708,10 +5713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EC1B12-8D19-48E1-AE18-CC4CE60CD15C}">
-  <dimension ref="B9:R57"/>
+  <dimension ref="A9:R60"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5723,7 +5728,7 @@
     <col min="14" max="14" width="9.7109375" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="2:18">
+    <row r="9" spans="1:18">
       <c r="G9" t="s">
         <v>1062</v>
       </c>
@@ -5734,13 +5739,16 @@
       </c>
       <c r="M9" s="1">
         <f ca="1">TODAY()</f>
-        <v>44730</v>
+        <v>44734</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>1061</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="77.25">
+    <row r="10" spans="1:18" ht="77.25">
+      <c r="A10" t="s">
+        <v>1123</v>
+      </c>
       <c r="K10" t="s">
         <v>11</v>
       </c>
@@ -5761,7 +5769,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="11" spans="2:18">
+    <row r="11" spans="1:18">
       <c r="B11" s="1">
         <v>44714</v>
       </c>
@@ -5799,14 +5807,14 @@
       </c>
       <c r="Q11" s="16">
         <f>AVERAGE(Q26:Q60)</f>
-        <v>2.4151005043421565E-3</v>
+        <v>2.3281516042127394E-3</v>
       </c>
       <c r="R11" s="16">
         <f>(1+Q11)^92</f>
-        <v>1.2484732102101657</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18">
+        <v>1.2385495789168448</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="B12" s="1">
         <v>44714</v>
       </c>
@@ -5839,7 +5847,7 @@
         <v>-5097.28</v>
       </c>
     </row>
-    <row r="13" spans="2:18">
+    <row r="13" spans="1:18">
       <c r="B13" s="1">
         <v>44717</v>
       </c>
@@ -5871,7 +5879,7 @@
         <v>4922.5199999999995</v>
       </c>
     </row>
-    <row r="14" spans="2:18">
+    <row r="14" spans="1:18">
       <c r="B14" s="1">
         <v>44717</v>
       </c>
@@ -5903,7 +5911,7 @@
         <v>5012.32</v>
       </c>
     </row>
-    <row r="15" spans="2:18">
+    <row r="15" spans="1:18">
       <c r="B15" s="1">
         <v>44719</v>
       </c>
@@ -5935,7 +5943,7 @@
         <v>-1068.18</v>
       </c>
     </row>
-    <row r="16" spans="2:18">
+    <row r="16" spans="1:18">
       <c r="B16" s="1">
         <v>44719</v>
       </c>
@@ -6230,7 +6238,7 @@
       </c>
       <c r="N24" s="28">
         <f ca="1">$M$9-M24</f>
-        <v>-33</v>
+        <v>-29</v>
       </c>
     </row>
     <row r="25" spans="2:18">
@@ -6272,7 +6280,7 @@
       </c>
       <c r="N25" s="28">
         <f ca="1">$M$9-M25</f>
-        <v>-19</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="26" spans="2:18">
@@ -6317,7 +6325,7 @@
       </c>
       <c r="N26" s="28">
         <f t="shared" ref="N26:N51" ca="1" si="5">$M$9-M26</f>
-        <v>-78</v>
+        <v>-74</v>
       </c>
       <c r="O26">
         <v>0.1</v>
@@ -6377,7 +6385,7 @@
       </c>
       <c r="N27" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-36</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="28" spans="2:18">
@@ -6422,7 +6430,7 @@
       </c>
       <c r="N28" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-36</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="29" spans="2:18">
@@ -6467,13 +6475,13 @@
       </c>
       <c r="N29" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O29">
         <v>0.41</v>
       </c>
       <c r="P29" s="16">
-        <f t="shared" ref="P29:P57" si="10">M29-B29</f>
+        <f t="shared" ref="P29:P58" si="10">M29-B29</f>
         <v>91</v>
       </c>
       <c r="Q29" s="16">
@@ -6527,7 +6535,7 @@
       </c>
       <c r="N30" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-57</v>
+        <v>-53</v>
       </c>
       <c r="O30">
         <v>0.13400000000000001</v>
@@ -6587,7 +6595,7 @@
       </c>
       <c r="N31" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-67</v>
       </c>
       <c r="O31">
         <v>0.17</v>
@@ -6647,7 +6655,7 @@
       </c>
       <c r="N32" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-67</v>
       </c>
       <c r="O32">
         <v>0.12</v>
@@ -6707,7 +6715,7 @@
       </c>
       <c r="N33" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-67</v>
       </c>
       <c r="O33">
         <v>0.13200000000000001</v>
@@ -6767,7 +6775,7 @@
       </c>
       <c r="N34" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-36</v>
+        <v>-32</v>
       </c>
       <c r="O34">
         <v>9.9000000000000005E-2</v>
@@ -6827,7 +6835,7 @@
       </c>
       <c r="N35" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O35">
         <v>0.12</v>
@@ -6887,7 +6895,7 @@
       </c>
       <c r="N36" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O36">
         <v>0.14000000000000001</v>
@@ -6947,7 +6955,7 @@
       </c>
       <c r="N37" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O37">
         <v>0.35</v>
@@ -7007,7 +7015,7 @@
       </c>
       <c r="N38" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O38" s="18">
         <v>0.28000000000000003</v>
@@ -7067,7 +7075,7 @@
       </c>
       <c r="N39" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-15</v>
+        <v>-11</v>
       </c>
       <c r="O39">
         <v>0.11</v>
@@ -7127,7 +7135,7 @@
       </c>
       <c r="N40" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O40" s="18">
         <v>0.11</v>
@@ -7187,7 +7195,7 @@
       </c>
       <c r="N41" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O41">
         <v>9.6000000000000002E-2</v>
@@ -7247,7 +7255,7 @@
       </c>
       <c r="N42" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O42">
         <v>0.22</v>
@@ -7307,7 +7315,7 @@
       </c>
       <c r="N43" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O43">
         <v>0.73</v>
@@ -7367,7 +7375,7 @@
       </c>
       <c r="N44" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O44" s="18">
         <v>0.26500000000000001</v>
@@ -7427,7 +7435,7 @@
       </c>
       <c r="N45" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O45">
         <v>0.13</v>
@@ -7487,7 +7495,7 @@
       </c>
       <c r="N46" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O46">
         <v>0.16</v>
@@ -7547,7 +7555,7 @@
       </c>
       <c r="N47" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O47" s="18">
         <v>0.09</v>
@@ -7607,7 +7615,7 @@
       </c>
       <c r="N48" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O48" s="18">
         <v>0.3</v>
@@ -7625,7 +7633,7 @@
         <v>1.3037534691790746</v>
       </c>
     </row>
-    <row r="49" spans="2:18">
+    <row r="49" spans="1:18">
       <c r="B49" s="1">
         <v>44724</v>
       </c>
@@ -7667,7 +7675,7 @@
       </c>
       <c r="N49" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-67</v>
       </c>
       <c r="O49">
         <v>0.12</v>
@@ -7685,7 +7693,7 @@
         <v>1.1450012193329568</v>
       </c>
     </row>
-    <row r="50" spans="2:18">
+    <row r="50" spans="1:18">
       <c r="B50" s="1">
         <v>44724</v>
       </c>
@@ -7727,7 +7735,7 @@
       </c>
       <c r="N50" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-50</v>
+        <v>-46</v>
       </c>
       <c r="O50">
         <v>9.4899999999999998E-2</v>
@@ -7745,7 +7753,7 @@
         <v>1.1606107956028482</v>
       </c>
     </row>
-    <row r="51" spans="2:18">
+    <row r="51" spans="1:18">
       <c r="B51" s="1">
         <v>44724</v>
       </c>
@@ -7766,7 +7774,7 @@
         <v>155.49</v>
       </c>
       <c r="H51" s="18">
-        <f t="shared" ref="H51:H57" si="18">G51*E51</f>
+        <f t="shared" ref="H51:H58" si="18">G51*E51</f>
         <v>1088.43</v>
       </c>
       <c r="I51" s="19">
@@ -7787,7 +7795,7 @@
       </c>
       <c r="N51" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-85</v>
+        <v>-81</v>
       </c>
       <c r="O51">
         <v>0.14000000000000001</v>
@@ -7805,7 +7813,7 @@
         <v>1.1416426352652658</v>
       </c>
     </row>
-    <row r="52" spans="2:18">
+    <row r="52" spans="1:18">
       <c r="B52" s="1">
         <v>44729</v>
       </c>
@@ -7820,7 +7828,7 @@
       </c>
       <c r="F52" s="27" cm="1">
         <f t="array" ref="F52">SUMPRODUCT(($C$11:$C$100=C52)*($E$11:$E$100))</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="G52">
         <v>17.97</v>
@@ -7847,7 +7855,7 @@
       </c>
       <c r="N52" s="28">
         <f t="shared" ref="N52" ca="1" si="21">$M$9-M52</f>
-        <v>-22</v>
+        <v>-18</v>
       </c>
       <c r="O52" s="27">
         <v>0.16561899999999999</v>
@@ -7865,7 +7873,7 @@
         <v>1.8459777917460405</v>
       </c>
     </row>
-    <row r="53" spans="2:18">
+    <row r="53" spans="1:18">
       <c r="B53" s="1">
         <v>44729</v>
       </c>
@@ -7907,7 +7915,7 @@
       </c>
       <c r="N53" s="28">
         <f t="shared" ref="N53" ca="1" si="25">$M$9-M53</f>
-        <v>-92</v>
+        <v>-88</v>
       </c>
       <c r="O53" s="27">
         <v>0.44709700000000002</v>
@@ -7925,7 +7933,7 @@
         <v>1.4413579971829127</v>
       </c>
     </row>
-    <row r="54" spans="2:18">
+    <row r="54" spans="1:18">
       <c r="B54" s="1">
         <v>44729</v>
       </c>
@@ -7966,8 +7974,8 @@
         <v>44794</v>
       </c>
       <c r="N54" s="28">
-        <f t="shared" ref="N54:N57" ca="1" si="29">$M$9-M54</f>
-        <v>-64</v>
+        <f t="shared" ref="N54:N58" ca="1" si="29">$M$9-M54</f>
+        <v>-60</v>
       </c>
       <c r="O54" s="27">
         <v>0.44709700000000002</v>
@@ -7985,7 +7993,7 @@
         <v>1.6871973902345887</v>
       </c>
     </row>
-    <row r="55" spans="2:18">
+    <row r="55" spans="1:18">
       <c r="B55" s="1">
         <v>44729</v>
       </c>
@@ -8027,7 +8035,7 @@
       </c>
       <c r="N55" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-50</v>
+        <v>-46</v>
       </c>
       <c r="O55" s="27">
         <v>7.9225000000000004E-2</v>
@@ -8045,7 +8053,7 @@
         <v>1.1474438584033493</v>
       </c>
     </row>
-    <row r="56" spans="2:18">
+    <row r="56" spans="1:18">
       <c r="B56" s="1">
         <v>44729</v>
       </c>
@@ -8087,7 +8095,7 @@
       </c>
       <c r="N56" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-36</v>
+        <v>-32</v>
       </c>
       <c r="O56" s="27">
         <v>4.7683999999999997E-2</v>
@@ -8105,7 +8113,7 @@
         <v>1.122799979907529</v>
       </c>
     </row>
-    <row r="57" spans="2:18">
+    <row r="57" spans="1:18">
       <c r="B57" s="1">
         <v>44729</v>
       </c>
@@ -8147,7 +8155,7 @@
       </c>
       <c r="N57" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-29</v>
+        <v>-25</v>
       </c>
       <c r="O57" s="27">
         <v>3.1424000000000001E-2</v>
@@ -8157,17 +8165,202 @@
         <v>30</v>
       </c>
       <c r="Q57" s="27">
-        <f t="shared" ref="Q57" si="39">(1+O57)^(1/P57)-1</f>
+        <f t="shared" ref="Q57:Q58" si="39">(1+O57)^(1/P57)-1</f>
         <v>1.0318777434383808E-3</v>
       </c>
       <c r="R57" s="27">
-        <f t="shared" ref="R57" si="40">(1+Q57)^92</f>
+        <f t="shared" ref="R57:R58" si="40">(1+Q57)^92</f>
         <v>1.0995310894115367</v>
       </c>
     </row>
+    <row r="58" spans="1:18">
+      <c r="B58" s="1">
+        <v>44730</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D58" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>60</v>
+      </c>
+      <c r="F58" s="19" cm="1">
+        <f t="array" ref="F58">SUMPRODUCT(($C$11:$C$100=C58)*($E$11:$E$100))</f>
+        <v>120</v>
+      </c>
+      <c r="G58">
+        <v>17.97</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="18"/>
+        <v>1078.1999999999998</v>
+      </c>
+      <c r="I58" s="32">
+        <v>-1</v>
+      </c>
+      <c r="J58" s="32">
+        <f t="shared" ref="J58" si="41">I58*H58</f>
+        <v>-1078.1999999999998</v>
+      </c>
+      <c r="K58" t="s">
+        <v>1064</v>
+      </c>
+      <c r="L58" t="s">
+        <v>142</v>
+      </c>
+      <c r="M58" s="1">
+        <v>44766</v>
+      </c>
+      <c r="N58" s="28">
+        <f t="shared" ca="1" si="29"/>
+        <v>-32</v>
+      </c>
+      <c r="O58" s="32">
+        <v>2.7649E-2</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="10"/>
+        <v>36</v>
+      </c>
+      <c r="Q58" s="32">
+        <f t="shared" ref="Q58" si="42">(1+O58)^(1/P58)-1</f>
+        <v>7.5788897060924398E-4</v>
+      </c>
+      <c r="R58" s="32">
+        <f t="shared" ref="R58" si="43">(1+Q58)^92</f>
+        <v>1.0721858084819609</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
+      <c r="A59">
+        <v>202</v>
+      </c>
+      <c r="B59" s="1">
+        <v>44734</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>5</v>
+      </c>
+      <c r="F59" s="19" cm="1">
+        <f t="array" ref="F59">SUMPRODUCT(($C$11:$C$100=C59)*($E$11:$E$100))</f>
+        <v>5</v>
+      </c>
+      <c r="G59">
+        <v>208.52</v>
+      </c>
+      <c r="H59">
+        <f>G59*E59</f>
+        <v>1042.6000000000001</v>
+      </c>
+      <c r="I59" s="31">
+        <v>-1</v>
+      </c>
+      <c r="J59" s="31">
+        <f t="shared" ref="J59" si="44">I59*H59</f>
+        <v>-1042.6000000000001</v>
+      </c>
+      <c r="K59" t="s">
+        <v>1100</v>
+      </c>
+      <c r="M59" s="1">
+        <v>44782</v>
+      </c>
+      <c r="N59" s="28">
+        <f ca="1">$M$9-M59</f>
+        <v>-48</v>
+      </c>
+      <c r="O59">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="P59">
+        <f>M59-B59</f>
+        <v>48</v>
+      </c>
+      <c r="Q59">
+        <f>(1+O59)^(1/P59)-1</f>
+        <v>1.3519750186554713E-3</v>
+      </c>
+      <c r="R59">
+        <f>(1+Q59)^92</f>
+        <v>1.1323529188332864</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
+      <c r="A60">
+        <v>37</v>
+      </c>
+      <c r="B60" s="1">
+        <v>44734</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D60" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>25</v>
+      </c>
+      <c r="F60" s="19" cm="1">
+        <f t="array" ref="F60">SUMPRODUCT(($C$11:$C$100=C60)*($E$11:$E$100))</f>
+        <v>25</v>
+      </c>
+      <c r="G60">
+        <v>40.15</v>
+      </c>
+      <c r="H60">
+        <f>G60*E60</f>
+        <v>1003.75</v>
+      </c>
+      <c r="I60" s="32">
+        <v>-1</v>
+      </c>
+      <c r="J60" s="32">
+        <f t="shared" ref="J60" si="45">I60*H60</f>
+        <v>-1003.75</v>
+      </c>
+      <c r="K60" s="32" t="s">
+        <v>1100</v>
+      </c>
+      <c r="M60" s="1">
+        <v>44768</v>
+      </c>
+      <c r="N60" s="28">
+        <f ca="1">$M$9-M60</f>
+        <v>-34</v>
+      </c>
+      <c r="O60">
+        <v>0.08</v>
+      </c>
+      <c r="P60">
+        <f>M60-B60</f>
+        <v>34</v>
+      </c>
+      <c r="Q60">
+        <f>(1+O60)^(1/P60)-1</f>
+        <v>2.2661238194909838E-3</v>
+      </c>
+      <c r="R60">
+        <f>(1+Q60)^92</f>
+        <v>1.2315179609375255</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="Q26:Q57">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="N24:N60">
+    <cfRule type="expression" priority="1">
+      <formula>"&gt;=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q26:Q60">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -8176,11 +8369,6 @@
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N24:N57">
-    <cfRule type="expression" priority="1">
-      <formula>"&gt;=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8431,10 +8619,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="32"/>
+      <c r="B35" s="34"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -8491,10 +8679,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="32"/>
+      <c r="B44" s="34"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -8980,10 +9168,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="32"/>
+      <c r="B38" s="34"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6"/>
@@ -9040,10 +9228,10 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="32"/>
+      <c r="B47" s="34"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6"/>
@@ -10426,10 +10614,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="32"/>
+      <c r="B38" s="34"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="6"/>
@@ -10486,10 +10674,10 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="32"/>
+      <c r="B47" s="34"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="6"/>
@@ -10812,10 +11000,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="32"/>
+      <c r="B35" s="34"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -10872,10 +11060,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="32"/>
+      <c r="B44" s="34"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -11372,10 +11560,10 @@
       <c r="A14" s="10"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="32"/>
+      <c r="B15" s="34"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6"/>
@@ -11432,10 +11620,10 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="32"/>
+      <c r="B24" s="34"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6"/>
@@ -11750,10 +11938,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="32"/>
+      <c r="B32" s="34"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -11810,10 +11998,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="32"/>
+      <c r="B41" s="34"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -12098,8 +12286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5B5641-1C14-45B9-9884-6F6125221349}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15544,10 +15732,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="32"/>
+      <c r="B35" s="34"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -15604,10 +15792,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="32"/>
+      <c r="B44" s="34"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -15935,10 +16123,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="32"/>
+      <c r="B35" s="34"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -15995,10 +16183,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="32"/>
+      <c r="B44" s="34"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -17138,10 +17326,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="32"/>
+      <c r="B35" s="34"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -17198,10 +17386,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="32"/>
+      <c r="B44" s="34"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -17814,10 +18002,10 @@
       <c r="A62" s="10"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="31" t="s">
+      <c r="A63" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="32"/>
+      <c r="B63" s="34"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6"/>
@@ -17874,10 +18062,10 @@
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="31" t="s">
+      <c r="A72" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B72" s="32"/>
+      <c r="B72" s="34"/>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="6"/>
@@ -18337,10 +18525,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="32"/>
+      <c r="B32" s="34"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -18397,10 +18585,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="32"/>
+      <c r="B41" s="34"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -19488,10 +19676,10 @@
       <c r="A31" s="22"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="32"/>
+      <c r="B32" s="34"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="12"/>
@@ -19548,10 +19736,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="32"/>
+      <c r="B41" s="34"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="12"/>

</xml_diff>

<commit_message>
revisions to analyzesp1500 and sp1500
added
'USALOLITONOSTSAM','USPHCI'
</commit_message>
<xml_diff>
--- a/code/Screener/record.xlsx
+++ b/code/Screener/record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CCBBB0-6A95-4BA7-A98E-8B93B69BC0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12465F05-F3E4-481F-8410-D7D91440630A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
@@ -5715,8 +5715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EC1B12-8D19-48E1-AE18-CC4CE60CD15C}">
   <dimension ref="A9:R60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26:P60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5739,7 +5739,7 @@
       </c>
       <c r="M9" s="1">
         <f ca="1">TODAY()</f>
-        <v>44734</v>
+        <v>44739</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>1061</v>
@@ -6238,7 +6238,7 @@
       </c>
       <c r="N24" s="28">
         <f ca="1">$M$9-M24</f>
-        <v>-29</v>
+        <v>-24</v>
       </c>
     </row>
     <row r="25" spans="2:18">
@@ -6280,7 +6280,7 @@
       </c>
       <c r="N25" s="28">
         <f ca="1">$M$9-M25</f>
-        <v>-15</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="26" spans="2:18">
@@ -6325,7 +6325,7 @@
       </c>
       <c r="N26" s="28">
         <f t="shared" ref="N26:N51" ca="1" si="5">$M$9-M26</f>
-        <v>-74</v>
+        <v>-69</v>
       </c>
       <c r="O26">
         <v>0.1</v>
@@ -6385,7 +6385,7 @@
       </c>
       <c r="N27" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-32</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="28" spans="2:18">
@@ -6430,7 +6430,7 @@
       </c>
       <c r="N28" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-32</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="29" spans="2:18">
@@ -6475,7 +6475,7 @@
       </c>
       <c r="N29" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O29">
         <v>0.41</v>
@@ -6535,7 +6535,7 @@
       </c>
       <c r="N30" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-53</v>
+        <v>-48</v>
       </c>
       <c r="O30">
         <v>0.13400000000000001</v>
@@ -6595,7 +6595,7 @@
       </c>
       <c r="N31" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-67</v>
+        <v>-62</v>
       </c>
       <c r="O31">
         <v>0.17</v>
@@ -6655,7 +6655,7 @@
       </c>
       <c r="N32" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-67</v>
+        <v>-62</v>
       </c>
       <c r="O32">
         <v>0.12</v>
@@ -6715,7 +6715,7 @@
       </c>
       <c r="N33" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-67</v>
+        <v>-62</v>
       </c>
       <c r="O33">
         <v>0.13200000000000001</v>
@@ -6775,7 +6775,7 @@
       </c>
       <c r="N34" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-32</v>
+        <v>-27</v>
       </c>
       <c r="O34">
         <v>9.9000000000000005E-2</v>
@@ -6835,7 +6835,7 @@
       </c>
       <c r="N35" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O35">
         <v>0.12</v>
@@ -6895,7 +6895,7 @@
       </c>
       <c r="N36" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O36">
         <v>0.14000000000000001</v>
@@ -6955,7 +6955,7 @@
       </c>
       <c r="N37" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O37">
         <v>0.35</v>
@@ -7015,7 +7015,7 @@
       </c>
       <c r="N38" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O38" s="18">
         <v>0.28000000000000003</v>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="N39" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-11</v>
+        <v>-6</v>
       </c>
       <c r="O39">
         <v>0.11</v>
@@ -7135,7 +7135,7 @@
       </c>
       <c r="N40" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O40" s="18">
         <v>0.11</v>
@@ -7195,7 +7195,7 @@
       </c>
       <c r="N41" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O41">
         <v>9.6000000000000002E-2</v>
@@ -7255,7 +7255,7 @@
       </c>
       <c r="N42" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O42">
         <v>0.22</v>
@@ -7315,7 +7315,7 @@
       </c>
       <c r="N43" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O43">
         <v>0.73</v>
@@ -7375,7 +7375,7 @@
       </c>
       <c r="N44" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O44" s="18">
         <v>0.26500000000000001</v>
@@ -7435,7 +7435,7 @@
       </c>
       <c r="N45" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O45">
         <v>0.13</v>
@@ -7495,7 +7495,7 @@
       </c>
       <c r="N46" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O46">
         <v>0.16</v>
@@ -7555,7 +7555,7 @@
       </c>
       <c r="N47" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O47" s="18">
         <v>0.09</v>
@@ -7615,7 +7615,7 @@
       </c>
       <c r="N48" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O48" s="18">
         <v>0.3</v>
@@ -7675,7 +7675,7 @@
       </c>
       <c r="N49" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-67</v>
+        <v>-62</v>
       </c>
       <c r="O49">
         <v>0.12</v>
@@ -7735,7 +7735,7 @@
       </c>
       <c r="N50" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-46</v>
+        <v>-41</v>
       </c>
       <c r="O50">
         <v>9.4899999999999998E-2</v>
@@ -7795,7 +7795,7 @@
       </c>
       <c r="N51" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-81</v>
+        <v>-76</v>
       </c>
       <c r="O51">
         <v>0.14000000000000001</v>
@@ -7855,7 +7855,7 @@
       </c>
       <c r="N52" s="28">
         <f t="shared" ref="N52" ca="1" si="21">$M$9-M52</f>
-        <v>-18</v>
+        <v>-13</v>
       </c>
       <c r="O52" s="27">
         <v>0.16561899999999999</v>
@@ -7915,7 +7915,7 @@
       </c>
       <c r="N53" s="28">
         <f t="shared" ref="N53" ca="1" si="25">$M$9-M53</f>
-        <v>-88</v>
+        <v>-83</v>
       </c>
       <c r="O53" s="27">
         <v>0.44709700000000002</v>
@@ -7975,7 +7975,7 @@
       </c>
       <c r="N54" s="28">
         <f t="shared" ref="N54:N58" ca="1" si="29">$M$9-M54</f>
-        <v>-60</v>
+        <v>-55</v>
       </c>
       <c r="O54" s="27">
         <v>0.44709700000000002</v>
@@ -8035,7 +8035,7 @@
       </c>
       <c r="N55" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-46</v>
+        <v>-41</v>
       </c>
       <c r="O55" s="27">
         <v>7.9225000000000004E-2</v>
@@ -8095,7 +8095,7 @@
       </c>
       <c r="N56" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-32</v>
+        <v>-27</v>
       </c>
       <c r="O56" s="27">
         <v>4.7683999999999997E-2</v>
@@ -8155,7 +8155,7 @@
       </c>
       <c r="N57" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-25</v>
+        <v>-20</v>
       </c>
       <c r="O57" s="27">
         <v>3.1424000000000001E-2</v>
@@ -8165,11 +8165,11 @@
         <v>30</v>
       </c>
       <c r="Q57" s="27">
-        <f t="shared" ref="Q57:Q58" si="39">(1+O57)^(1/P57)-1</f>
+        <f t="shared" ref="Q57" si="39">(1+O57)^(1/P57)-1</f>
         <v>1.0318777434383808E-3</v>
       </c>
       <c r="R57" s="27">
-        <f t="shared" ref="R57:R58" si="40">(1+Q57)^92</f>
+        <f t="shared" ref="R57" si="40">(1+Q57)^92</f>
         <v>1.0995310894115367</v>
       </c>
     </row>
@@ -8215,7 +8215,7 @@
       </c>
       <c r="N58" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-32</v>
+        <v>-27</v>
       </c>
       <c r="O58" s="32">
         <v>2.7649E-2</v>
@@ -8275,7 +8275,7 @@
       </c>
       <c r="N59" s="28">
         <f ca="1">$M$9-M59</f>
-        <v>-48</v>
+        <v>-43</v>
       </c>
       <c r="O59">
         <v>6.7000000000000004E-2</v>
@@ -8335,7 +8335,7 @@
       </c>
       <c r="N60" s="28">
         <f ca="1">$M$9-M60</f>
-        <v>-34</v>
+        <v>-29</v>
       </c>
       <c r="O60">
         <v>0.08</v>
@@ -8355,12 +8355,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N24:N60">
-    <cfRule type="expression" priority="1">
+    <cfRule type="expression" priority="2">
       <formula>"&gt;=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q26:Q60">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P26:P60">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
v 9.0.2 ensured analyzesp1500 worked
</commit_message>
<xml_diff>
--- a/code/Screener/record.xlsx
+++ b/code/Screener/record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12465F05-F3E4-481F-8410-D7D91440630A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76737857-0CC6-46B8-A829-4F47E858ADAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2005" uniqueCount="1125">
   <si>
     <t>EXC</t>
   </si>
@@ -3444,6 +3444,9 @@
   </si>
   <si>
     <t>Stop Loss</t>
+  </si>
+  <si>
+    <t>yea</t>
   </si>
 </sst>
 </file>
@@ -3550,7 +3553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3624,6 +3627,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5713,10 +5717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EC1B12-8D19-48E1-AE18-CC4CE60CD15C}">
-  <dimension ref="A9:R60"/>
+  <dimension ref="A9:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26:P60"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61:J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5739,7 +5743,7 @@
       </c>
       <c r="M9" s="1">
         <f ca="1">TODAY()</f>
-        <v>44739</v>
+        <v>44741</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>1061</v>
@@ -5803,15 +5807,15 @@
       </c>
       <c r="P11">
         <f>AVERAGE(P26:P32)</f>
-        <v>78.400000000000006</v>
-      </c>
-      <c r="Q11" s="16">
+        <v>77</v>
+      </c>
+      <c r="Q11" s="16" t="e">
         <f>AVERAGE(Q26:Q60)</f>
-        <v>2.3281516042127394E-3</v>
-      </c>
-      <c r="R11" s="16">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R11" s="16" t="e">
         <f>(1+Q11)^92</f>
-        <v>1.2385495789168448</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -6238,7 +6242,7 @@
       </c>
       <c r="N24" s="28">
         <f ca="1">$M$9-M24</f>
-        <v>-24</v>
+        <v>-22</v>
       </c>
     </row>
     <row r="25" spans="2:18">
@@ -6280,7 +6284,7 @@
       </c>
       <c r="N25" s="28">
         <f ca="1">$M$9-M25</f>
-        <v>-10</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="26" spans="2:18">
@@ -6325,22 +6329,21 @@
       </c>
       <c r="N26" s="28">
         <f t="shared" ref="N26:N51" ca="1" si="5">$M$9-M26</f>
-        <v>-69</v>
+        <v>-67</v>
       </c>
       <c r="O26">
         <v>0.1</v>
       </c>
-      <c r="P26" s="16">
-        <f>M26-B26</f>
-        <v>84</v>
-      </c>
-      <c r="Q26" s="16">
+      <c r="P26" s="16" t="s">
+        <v>1124</v>
+      </c>
+      <c r="Q26" s="16" t="e">
         <f>(1+O26)^(1/P26)-1</f>
-        <v>1.135288950835589E-3</v>
-      </c>
-      <c r="R26" s="16">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R26" s="16" t="e">
         <f>(1+Q26)^92</f>
-        <v>1.1100303305665855</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="27" spans="2:18">
@@ -6385,7 +6388,7 @@
       </c>
       <c r="N27" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-27</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="28" spans="2:18">
@@ -6430,7 +6433,7 @@
       </c>
       <c r="N28" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-27</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="29" spans="2:18">
@@ -6475,7 +6478,7 @@
       </c>
       <c r="N29" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O29">
         <v>0.41</v>
@@ -6535,7 +6538,7 @@
       </c>
       <c r="N30" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-48</v>
+        <v>-46</v>
       </c>
       <c r="O30">
         <v>0.13400000000000001</v>
@@ -6595,7 +6598,7 @@
       </c>
       <c r="N31" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-62</v>
+        <v>-60</v>
       </c>
       <c r="O31">
         <v>0.17</v>
@@ -6655,7 +6658,7 @@
       </c>
       <c r="N32" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-62</v>
+        <v>-60</v>
       </c>
       <c r="O32">
         <v>0.12</v>
@@ -6715,7 +6718,7 @@
       </c>
       <c r="N33" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-62</v>
+        <v>-60</v>
       </c>
       <c r="O33">
         <v>0.13200000000000001</v>
@@ -6775,7 +6778,7 @@
       </c>
       <c r="N34" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-27</v>
+        <v>-25</v>
       </c>
       <c r="O34">
         <v>9.9000000000000005E-2</v>
@@ -6835,7 +6838,7 @@
       </c>
       <c r="N35" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O35">
         <v>0.12</v>
@@ -6895,7 +6898,7 @@
       </c>
       <c r="N36" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O36">
         <v>0.14000000000000001</v>
@@ -6955,7 +6958,7 @@
       </c>
       <c r="N37" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O37">
         <v>0.35</v>
@@ -7015,7 +7018,7 @@
       </c>
       <c r="N38" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O38" s="18">
         <v>0.28000000000000003</v>
@@ -7075,7 +7078,7 @@
       </c>
       <c r="N39" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="O39">
         <v>0.11</v>
@@ -7135,7 +7138,7 @@
       </c>
       <c r="N40" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O40" s="18">
         <v>0.11</v>
@@ -7195,7 +7198,7 @@
       </c>
       <c r="N41" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O41">
         <v>9.6000000000000002E-2</v>
@@ -7255,7 +7258,7 @@
       </c>
       <c r="N42" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O42">
         <v>0.22</v>
@@ -7315,7 +7318,7 @@
       </c>
       <c r="N43" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O43">
         <v>0.73</v>
@@ -7375,7 +7378,7 @@
       </c>
       <c r="N44" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O44" s="18">
         <v>0.26500000000000001</v>
@@ -7435,7 +7438,7 @@
       </c>
       <c r="N45" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O45">
         <v>0.13</v>
@@ -7495,7 +7498,7 @@
       </c>
       <c r="N46" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O46">
         <v>0.16</v>
@@ -7555,7 +7558,7 @@
       </c>
       <c r="N47" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O47" s="18">
         <v>0.09</v>
@@ -7615,7 +7618,7 @@
       </c>
       <c r="N48" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O48" s="18">
         <v>0.3</v>
@@ -7675,7 +7678,7 @@
       </c>
       <c r="N49" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-62</v>
+        <v>-60</v>
       </c>
       <c r="O49">
         <v>0.12</v>
@@ -7735,7 +7738,7 @@
       </c>
       <c r="N50" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-41</v>
+        <v>-39</v>
       </c>
       <c r="O50">
         <v>9.4899999999999998E-2</v>
@@ -7795,7 +7798,7 @@
       </c>
       <c r="N51" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-76</v>
+        <v>-74</v>
       </c>
       <c r="O51">
         <v>0.14000000000000001</v>
@@ -7855,7 +7858,7 @@
       </c>
       <c r="N52" s="28">
         <f t="shared" ref="N52" ca="1" si="21">$M$9-M52</f>
-        <v>-13</v>
+        <v>-11</v>
       </c>
       <c r="O52" s="27">
         <v>0.16561899999999999</v>
@@ -7915,7 +7918,7 @@
       </c>
       <c r="N53" s="28">
         <f t="shared" ref="N53" ca="1" si="25">$M$9-M53</f>
-        <v>-83</v>
+        <v>-81</v>
       </c>
       <c r="O53" s="27">
         <v>0.44709700000000002</v>
@@ -7975,7 +7978,7 @@
       </c>
       <c r="N54" s="28">
         <f t="shared" ref="N54:N58" ca="1" si="29">$M$9-M54</f>
-        <v>-55</v>
+        <v>-53</v>
       </c>
       <c r="O54" s="27">
         <v>0.44709700000000002</v>
@@ -8035,7 +8038,7 @@
       </c>
       <c r="N55" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-41</v>
+        <v>-39</v>
       </c>
       <c r="O55" s="27">
         <v>7.9225000000000004E-2</v>
@@ -8095,7 +8098,7 @@
       </c>
       <c r="N56" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-27</v>
+        <v>-25</v>
       </c>
       <c r="O56" s="27">
         <v>4.7683999999999997E-2</v>
@@ -8155,7 +8158,7 @@
       </c>
       <c r="N57" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-20</v>
+        <v>-18</v>
       </c>
       <c r="O57" s="27">
         <v>3.1424000000000001E-2</v>
@@ -8215,7 +8218,7 @@
       </c>
       <c r="N58" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-27</v>
+        <v>-25</v>
       </c>
       <c r="O58" s="32">
         <v>2.7649E-2</v>
@@ -8275,7 +8278,7 @@
       </c>
       <c r="N59" s="28">
         <f ca="1">$M$9-M59</f>
-        <v>-43</v>
+        <v>-41</v>
       </c>
       <c r="O59">
         <v>6.7000000000000004E-2</v>
@@ -8335,7 +8338,7 @@
       </c>
       <c r="N60" s="28">
         <f ca="1">$M$9-M60</f>
-        <v>-29</v>
+        <v>-27</v>
       </c>
       <c r="O60">
         <v>0.08</v>
@@ -8353,13 +8356,73 @@
         <v>1.2315179609375255</v>
       </c>
     </row>
+    <row r="61" spans="1:18">
+      <c r="B61" s="1">
+        <v>44741</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D61" t="s">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+      <c r="F61" s="19" cm="1">
+        <f t="array" ref="F61">SUMPRODUCT(($C$11:$C$100=C61)*($E$11:$E$100))</f>
+        <v>3</v>
+      </c>
+      <c r="G61">
+        <v>323</v>
+      </c>
+      <c r="H61">
+        <f>G61*E61</f>
+        <v>969</v>
+      </c>
+      <c r="I61" s="33">
+        <v>-1</v>
+      </c>
+      <c r="J61" s="33">
+        <f t="shared" ref="J61" si="46">I61*H61</f>
+        <v>-969</v>
+      </c>
+      <c r="K61" t="s">
+        <v>10</v>
+      </c>
+      <c r="L61" t="s">
+        <v>141</v>
+      </c>
+      <c r="M61" s="1">
+        <v>44838</v>
+      </c>
+      <c r="N61" s="28">
+        <f ca="1">$M$9-M61</f>
+        <v>-97</v>
+      </c>
+      <c r="O61">
+        <v>0.09</v>
+      </c>
+      <c r="P61">
+        <f>M61-B61</f>
+        <v>97</v>
+      </c>
+      <c r="Q61">
+        <f>(1+O61)^(1/P61)-1</f>
+        <v>8.8882462886163971E-4</v>
+      </c>
+      <c r="R61">
+        <f>(1+Q61)^92</f>
+        <v>1.0851687956828595</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="N24:N60">
+  <conditionalFormatting sqref="N24:N61">
     <cfRule type="expression" priority="2">
       <formula>"&gt;=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q26:Q60">
+  <conditionalFormatting sqref="Q26:Q61">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -8371,7 +8434,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P26:P60">
+  <conditionalFormatting sqref="P26:P61">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -8631,10 +8694,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="34"/>
+      <c r="B35" s="35"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -8691,10 +8754,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="33" t="s">
+      <c r="A44" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="34"/>
+      <c r="B44" s="35"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -9180,10 +9243,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="33" t="s">
+      <c r="A38" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="34"/>
+      <c r="B38" s="35"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6"/>
@@ -9240,10 +9303,10 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="34"/>
+      <c r="B47" s="35"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6"/>
@@ -10626,10 +10689,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="33" t="s">
+      <c r="A38" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="34"/>
+      <c r="B38" s="35"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="6"/>
@@ -10686,10 +10749,10 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="34"/>
+      <c r="B47" s="35"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="6"/>
@@ -11012,10 +11075,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="34"/>
+      <c r="B35" s="35"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -11072,10 +11135,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="33" t="s">
+      <c r="A44" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="34"/>
+      <c r="B44" s="35"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -11572,10 +11635,10 @@
       <c r="A14" s="10"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="34"/>
+      <c r="B15" s="35"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6"/>
@@ -11632,10 +11695,10 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="34"/>
+      <c r="B24" s="35"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6"/>
@@ -11950,10 +12013,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="34"/>
+      <c r="B32" s="35"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -12010,10 +12073,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="34"/>
+      <c r="B41" s="35"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -15744,10 +15807,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="34"/>
+      <c r="B35" s="35"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -15804,10 +15867,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="33" t="s">
+      <c r="A44" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="34"/>
+      <c r="B44" s="35"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -16135,10 +16198,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="34"/>
+      <c r="B35" s="35"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -16195,10 +16258,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="33" t="s">
+      <c r="A44" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="34"/>
+      <c r="B44" s="35"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -17338,10 +17401,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="34"/>
+      <c r="B35" s="35"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -17398,10 +17461,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="33" t="s">
+      <c r="A44" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="34"/>
+      <c r="B44" s="35"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -18014,10 +18077,10 @@
       <c r="A62" s="10"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="33" t="s">
+      <c r="A63" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="34"/>
+      <c r="B63" s="35"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6"/>
@@ -18074,10 +18137,10 @@
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="33" t="s">
+      <c r="A72" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="B72" s="34"/>
+      <c r="B72" s="35"/>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="6"/>
@@ -18537,10 +18600,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="34"/>
+      <c r="B32" s="35"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -18597,10 +18660,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="34"/>
+      <c r="B41" s="35"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -19688,10 +19751,10 @@
       <c r="A31" s="22"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="34"/>
+      <c r="B32" s="35"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="12"/>
@@ -19748,10 +19811,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="34"/>
+      <c r="B41" s="35"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="12"/>

</xml_diff>

<commit_message>
swapped ets for fbprophet forecasts
now I have more stocks I can trade with
</commit_message>
<xml_diff>
--- a/code/Screener/record.xlsx
+++ b/code/Screener/record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76737857-0CC6-46B8-A829-4F47E858ADAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56788FD7-2D1D-4C55-B921-9ED2751776F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
+    <workbookView xWindow="4470" yWindow="2760" windowWidth="20730" windowHeight="11835" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
   <sheets>
     <sheet name="Record book" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2005" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="1125">
   <si>
     <t>EXC</t>
   </si>
@@ -3553,7 +3553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3630,12 +3630,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5717,10 +5721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EC1B12-8D19-48E1-AE18-CC4CE60CD15C}">
-  <dimension ref="A9:R61"/>
+  <dimension ref="A9:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61:J61"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N62" sqref="N62:R62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5743,7 +5747,7 @@
       </c>
       <c r="M9" s="1">
         <f ca="1">TODAY()</f>
-        <v>44741</v>
+        <v>44743</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>1061</v>
@@ -6242,7 +6246,7 @@
       </c>
       <c r="N24" s="28">
         <f ca="1">$M$9-M24</f>
-        <v>-22</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="25" spans="2:18">
@@ -6284,7 +6288,7 @@
       </c>
       <c r="N25" s="28">
         <f ca="1">$M$9-M25</f>
-        <v>-8</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="26" spans="2:18">
@@ -6329,7 +6333,7 @@
       </c>
       <c r="N26" s="28">
         <f t="shared" ref="N26:N51" ca="1" si="5">$M$9-M26</f>
-        <v>-67</v>
+        <v>-65</v>
       </c>
       <c r="O26">
         <v>0.1</v>
@@ -6388,7 +6392,7 @@
       </c>
       <c r="N27" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-25</v>
+        <v>-23</v>
       </c>
     </row>
     <row r="28" spans="2:18">
@@ -6433,7 +6437,7 @@
       </c>
       <c r="N28" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-25</v>
+        <v>-23</v>
       </c>
     </row>
     <row r="29" spans="2:18">
@@ -6478,7 +6482,7 @@
       </c>
       <c r="N29" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O29">
         <v>0.41</v>
@@ -6538,7 +6542,7 @@
       </c>
       <c r="N30" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-46</v>
+        <v>-44</v>
       </c>
       <c r="O30">
         <v>0.13400000000000001</v>
@@ -6598,7 +6602,7 @@
       </c>
       <c r="N31" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-60</v>
+        <v>-58</v>
       </c>
       <c r="O31">
         <v>0.17</v>
@@ -6658,7 +6662,7 @@
       </c>
       <c r="N32" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-60</v>
+        <v>-58</v>
       </c>
       <c r="O32">
         <v>0.12</v>
@@ -6718,7 +6722,7 @@
       </c>
       <c r="N33" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-60</v>
+        <v>-58</v>
       </c>
       <c r="O33">
         <v>0.13200000000000001</v>
@@ -6778,7 +6782,7 @@
       </c>
       <c r="N34" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-25</v>
+        <v>-23</v>
       </c>
       <c r="O34">
         <v>9.9000000000000005E-2</v>
@@ -6838,7 +6842,7 @@
       </c>
       <c r="N35" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O35">
         <v>0.12</v>
@@ -6898,7 +6902,7 @@
       </c>
       <c r="N36" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O36">
         <v>0.14000000000000001</v>
@@ -6958,7 +6962,7 @@
       </c>
       <c r="N37" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O37">
         <v>0.35</v>
@@ -7018,7 +7022,7 @@
       </c>
       <c r="N38" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O38" s="18">
         <v>0.28000000000000003</v>
@@ -7078,7 +7082,7 @@
       </c>
       <c r="N39" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="O39">
         <v>0.11</v>
@@ -7138,7 +7142,7 @@
       </c>
       <c r="N40" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O40" s="18">
         <v>0.11</v>
@@ -7198,7 +7202,7 @@
       </c>
       <c r="N41" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O41">
         <v>9.6000000000000002E-2</v>
@@ -7258,7 +7262,7 @@
       </c>
       <c r="N42" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O42">
         <v>0.22</v>
@@ -7318,7 +7322,7 @@
       </c>
       <c r="N43" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O43">
         <v>0.73</v>
@@ -7378,7 +7382,7 @@
       </c>
       <c r="N44" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O44" s="18">
         <v>0.26500000000000001</v>
@@ -7438,7 +7442,7 @@
       </c>
       <c r="N45" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O45">
         <v>0.13</v>
@@ -7498,7 +7502,7 @@
       </c>
       <c r="N46" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O46">
         <v>0.16</v>
@@ -7558,7 +7562,7 @@
       </c>
       <c r="N47" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O47" s="18">
         <v>0.09</v>
@@ -7618,7 +7622,7 @@
       </c>
       <c r="N48" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O48" s="18">
         <v>0.3</v>
@@ -7678,7 +7682,7 @@
       </c>
       <c r="N49" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-60</v>
+        <v>-58</v>
       </c>
       <c r="O49">
         <v>0.12</v>
@@ -7738,7 +7742,7 @@
       </c>
       <c r="N50" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-39</v>
+        <v>-37</v>
       </c>
       <c r="O50">
         <v>9.4899999999999998E-2</v>
@@ -7798,7 +7802,7 @@
       </c>
       <c r="N51" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-74</v>
+        <v>-72</v>
       </c>
       <c r="O51">
         <v>0.14000000000000001</v>
@@ -7858,7 +7862,7 @@
       </c>
       <c r="N52" s="28">
         <f t="shared" ref="N52" ca="1" si="21">$M$9-M52</f>
-        <v>-11</v>
+        <v>-9</v>
       </c>
       <c r="O52" s="27">
         <v>0.16561899999999999</v>
@@ -7918,7 +7922,7 @@
       </c>
       <c r="N53" s="28">
         <f t="shared" ref="N53" ca="1" si="25">$M$9-M53</f>
-        <v>-81</v>
+        <v>-79</v>
       </c>
       <c r="O53" s="27">
         <v>0.44709700000000002</v>
@@ -7978,7 +7982,7 @@
       </c>
       <c r="N54" s="28">
         <f t="shared" ref="N54:N58" ca="1" si="29">$M$9-M54</f>
-        <v>-53</v>
+        <v>-51</v>
       </c>
       <c r="O54" s="27">
         <v>0.44709700000000002</v>
@@ -8038,7 +8042,7 @@
       </c>
       <c r="N55" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-39</v>
+        <v>-37</v>
       </c>
       <c r="O55" s="27">
         <v>7.9225000000000004E-2</v>
@@ -8098,7 +8102,7 @@
       </c>
       <c r="N56" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-25</v>
+        <v>-23</v>
       </c>
       <c r="O56" s="27">
         <v>4.7683999999999997E-2</v>
@@ -8158,7 +8162,7 @@
       </c>
       <c r="N57" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="O57" s="27">
         <v>3.1424000000000001E-2</v>
@@ -8218,7 +8222,7 @@
       </c>
       <c r="N58" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-25</v>
+        <v>-23</v>
       </c>
       <c r="O58" s="32">
         <v>2.7649E-2</v>
@@ -8278,7 +8282,7 @@
       </c>
       <c r="N59" s="28">
         <f ca="1">$M$9-M59</f>
-        <v>-41</v>
+        <v>-39</v>
       </c>
       <c r="O59">
         <v>6.7000000000000004E-2</v>
@@ -8338,7 +8342,7 @@
       </c>
       <c r="N60" s="28">
         <f ca="1">$M$9-M60</f>
-        <v>-27</v>
+        <v>-25</v>
       </c>
       <c r="O60">
         <v>0.08</v>
@@ -8398,7 +8402,7 @@
       </c>
       <c r="N61" s="28">
         <f ca="1">$M$9-M61</f>
-        <v>-97</v>
+        <v>-95</v>
       </c>
       <c r="O61">
         <v>0.09</v>
@@ -8416,13 +8420,73 @@
         <v>1.0851687956828595</v>
       </c>
     </row>
+    <row r="62" spans="1:18">
+      <c r="B62" s="1">
+        <v>44743</v>
+      </c>
+      <c r="C62" s="34" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D62" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>33</v>
+      </c>
+      <c r="F62" s="34" cm="1">
+        <f t="array" ref="F62">SUMPRODUCT(($C$11:$C$100=C62)*($E$11:$E$100))</f>
+        <v>33</v>
+      </c>
+      <c r="G62" s="34">
+        <v>31.5</v>
+      </c>
+      <c r="H62" s="34">
+        <f>G62*E62</f>
+        <v>1039.5</v>
+      </c>
+      <c r="I62" s="34">
+        <v>-1</v>
+      </c>
+      <c r="J62" s="34">
+        <f t="shared" ref="J62" si="47">I62*H62</f>
+        <v>-1039.5</v>
+      </c>
+      <c r="K62" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L62" t="s">
+        <v>142</v>
+      </c>
+      <c r="M62" s="38">
+        <v>44840</v>
+      </c>
+      <c r="N62" s="28">
+        <f ca="1">$M$9-M62</f>
+        <v>-97</v>
+      </c>
+      <c r="O62" s="34">
+        <v>0.09</v>
+      </c>
+      <c r="P62" s="34">
+        <f>M62-B62</f>
+        <v>97</v>
+      </c>
+      <c r="Q62" s="34">
+        <f>(1+O62)^(1/P62)-1</f>
+        <v>8.8882462886163971E-4</v>
+      </c>
+      <c r="R62" s="34">
+        <f>(1+Q62)^92</f>
+        <v>1.0851687956828595</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="N24:N61">
+  <conditionalFormatting sqref="N24:N62">
     <cfRule type="expression" priority="2">
       <formula>"&gt;=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q26:Q61">
+  <conditionalFormatting sqref="Q26:Q62">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -8434,7 +8498,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P26:P61">
+  <conditionalFormatting sqref="P26:P62">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -8694,10 +8758,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="36"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -8754,10 +8818,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="35"/>
+      <c r="B44" s="36"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -9243,10 +9307,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="35"/>
+      <c r="B38" s="36"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6"/>
@@ -9303,10 +9367,10 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="35"/>
+      <c r="B47" s="36"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6"/>
@@ -10689,10 +10753,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="35"/>
+      <c r="B38" s="36"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="6"/>
@@ -10749,10 +10813,10 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="35"/>
+      <c r="B47" s="36"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="6"/>
@@ -11075,10 +11139,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="36"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -11135,10 +11199,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="35"/>
+      <c r="B44" s="36"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -11635,10 +11699,10 @@
       <c r="A14" s="10"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="35"/>
+      <c r="B15" s="36"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6"/>
@@ -11695,10 +11759,10 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="36"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6"/>
@@ -12013,10 +12077,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="35"/>
+      <c r="B32" s="36"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -12073,10 +12137,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="35"/>
+      <c r="B41" s="36"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -15807,10 +15871,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="36"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -15867,10 +15931,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="35"/>
+      <c r="B44" s="36"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -16198,10 +16262,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="36"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -16258,10 +16322,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="35"/>
+      <c r="B44" s="36"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -17401,10 +17465,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="36"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -17461,10 +17525,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="35"/>
+      <c r="B44" s="36"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -18077,10 +18141,10 @@
       <c r="A62" s="10"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="34" t="s">
+      <c r="A63" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="35"/>
+      <c r="B63" s="36"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6"/>
@@ -18137,10 +18201,10 @@
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="34" t="s">
+      <c r="A72" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B72" s="35"/>
+      <c r="B72" s="36"/>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="6"/>
@@ -18600,10 +18664,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="35"/>
+      <c r="B32" s="36"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -18660,10 +18724,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="35"/>
+      <c r="B41" s="36"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -19751,10 +19815,10 @@
       <c r="A31" s="22"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="35"/>
+      <c r="B32" s="36"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="12"/>
@@ -19811,10 +19875,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="35"/>
+      <c r="B41" s="36"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="12"/>

</xml_diff>

<commit_message>
worked on fbprophet formula (mainly ensuring future dataframe had proper dates)
I'm getting inverted results from my former ets.  But I also did some changes with dates, so idk if I broke something, or I have bad results between former and now
</commit_message>
<xml_diff>
--- a/code/Screener/record.xlsx
+++ b/code/Screener/record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56788FD7-2D1D-4C55-B921-9ED2751776F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEB47A8-0FC5-4BBC-9F74-8D5F1EFEEB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="2760" windowWidth="20730" windowHeight="11835" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
+    <workbookView xWindow="4470" yWindow="2775" windowWidth="20730" windowHeight="11835" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
   <sheets>
     <sheet name="Record book" sheetId="1" r:id="rId1"/>
@@ -3553,7 +3553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3641,6 +3641,7 @@
     <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5721,10 +5722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EC1B12-8D19-48E1-AE18-CC4CE60CD15C}">
-  <dimension ref="A9:R62"/>
+  <dimension ref="A9:U62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N62" sqref="N62:R62"/>
+      <selection activeCell="U61" sqref="U61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5747,7 +5748,7 @@
       </c>
       <c r="M9" s="1">
         <f ca="1">TODAY()</f>
-        <v>44743</v>
+        <v>44744</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>1061</v>
@@ -6246,7 +6247,7 @@
       </c>
       <c r="N24" s="28">
         <f ca="1">$M$9-M24</f>
-        <v>-20</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="25" spans="2:18">
@@ -6288,7 +6289,7 @@
       </c>
       <c r="N25" s="28">
         <f ca="1">$M$9-M25</f>
-        <v>-6</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="26" spans="2:18">
@@ -6333,7 +6334,7 @@
       </c>
       <c r="N26" s="28">
         <f t="shared" ref="N26:N51" ca="1" si="5">$M$9-M26</f>
-        <v>-65</v>
+        <v>-64</v>
       </c>
       <c r="O26">
         <v>0.1</v>
@@ -6392,7 +6393,7 @@
       </c>
       <c r="N27" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-23</v>
+        <v>-22</v>
       </c>
     </row>
     <row r="28" spans="2:18">
@@ -6437,7 +6438,7 @@
       </c>
       <c r="N28" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-23</v>
+        <v>-22</v>
       </c>
     </row>
     <row r="29" spans="2:18">
@@ -6482,7 +6483,7 @@
       </c>
       <c r="N29" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O29">
         <v>0.41</v>
@@ -6542,7 +6543,7 @@
       </c>
       <c r="N30" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-44</v>
+        <v>-43</v>
       </c>
       <c r="O30">
         <v>0.13400000000000001</v>
@@ -6602,7 +6603,7 @@
       </c>
       <c r="N31" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-58</v>
+        <v>-57</v>
       </c>
       <c r="O31">
         <v>0.17</v>
@@ -6662,7 +6663,7 @@
       </c>
       <c r="N32" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-58</v>
+        <v>-57</v>
       </c>
       <c r="O32">
         <v>0.12</v>
@@ -6722,7 +6723,7 @@
       </c>
       <c r="N33" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-58</v>
+        <v>-57</v>
       </c>
       <c r="O33">
         <v>0.13200000000000001</v>
@@ -6782,7 +6783,7 @@
       </c>
       <c r="N34" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-23</v>
+        <v>-22</v>
       </c>
       <c r="O34">
         <v>9.9000000000000005E-2</v>
@@ -6842,7 +6843,7 @@
       </c>
       <c r="N35" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O35">
         <v>0.12</v>
@@ -6902,7 +6903,7 @@
       </c>
       <c r="N36" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O36">
         <v>0.14000000000000001</v>
@@ -6962,7 +6963,7 @@
       </c>
       <c r="N37" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O37">
         <v>0.35</v>
@@ -7022,7 +7023,7 @@
       </c>
       <c r="N38" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O38" s="18">
         <v>0.28000000000000003</v>
@@ -7082,7 +7083,7 @@
       </c>
       <c r="N39" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="O39">
         <v>0.11</v>
@@ -7142,7 +7143,7 @@
       </c>
       <c r="N40" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O40" s="18">
         <v>0.11</v>
@@ -7202,7 +7203,7 @@
       </c>
       <c r="N41" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O41">
         <v>9.6000000000000002E-2</v>
@@ -7262,7 +7263,7 @@
       </c>
       <c r="N42" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O42">
         <v>0.22</v>
@@ -7322,7 +7323,7 @@
       </c>
       <c r="N43" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O43">
         <v>0.73</v>
@@ -7382,7 +7383,7 @@
       </c>
       <c r="N44" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O44" s="18">
         <v>0.26500000000000001</v>
@@ -7442,7 +7443,7 @@
       </c>
       <c r="N45" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O45">
         <v>0.13</v>
@@ -7502,7 +7503,7 @@
       </c>
       <c r="N46" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O46">
         <v>0.16</v>
@@ -7562,7 +7563,7 @@
       </c>
       <c r="N47" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O47" s="18">
         <v>0.09</v>
@@ -7622,7 +7623,7 @@
       </c>
       <c r="N48" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O48" s="18">
         <v>0.3</v>
@@ -7640,7 +7641,7 @@
         <v>1.3037534691790746</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:21">
       <c r="B49" s="1">
         <v>44724</v>
       </c>
@@ -7682,7 +7683,7 @@
       </c>
       <c r="N49" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-58</v>
+        <v>-57</v>
       </c>
       <c r="O49">
         <v>0.12</v>
@@ -7700,7 +7701,7 @@
         <v>1.1450012193329568</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:21">
       <c r="B50" s="1">
         <v>44724</v>
       </c>
@@ -7742,7 +7743,7 @@
       </c>
       <c r="N50" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-37</v>
+        <v>-36</v>
       </c>
       <c r="O50">
         <v>9.4899999999999998E-2</v>
@@ -7760,7 +7761,7 @@
         <v>1.1606107956028482</v>
       </c>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:21">
       <c r="B51" s="1">
         <v>44724</v>
       </c>
@@ -7802,7 +7803,7 @@
       </c>
       <c r="N51" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="O51">
         <v>0.14000000000000001</v>
@@ -7820,7 +7821,7 @@
         <v>1.1416426352652658</v>
       </c>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:21">
       <c r="B52" s="1">
         <v>44729</v>
       </c>
@@ -7862,7 +7863,7 @@
       </c>
       <c r="N52" s="28">
         <f t="shared" ref="N52" ca="1" si="21">$M$9-M52</f>
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="O52" s="27">
         <v>0.16561899999999999</v>
@@ -7880,7 +7881,7 @@
         <v>1.8459777917460405</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:21">
       <c r="B53" s="1">
         <v>44729</v>
       </c>
@@ -7922,7 +7923,7 @@
       </c>
       <c r="N53" s="28">
         <f t="shared" ref="N53" ca="1" si="25">$M$9-M53</f>
-        <v>-79</v>
+        <v>-78</v>
       </c>
       <c r="O53" s="27">
         <v>0.44709700000000002</v>
@@ -7940,7 +7941,7 @@
         <v>1.4413579971829127</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:21">
       <c r="B54" s="1">
         <v>44729</v>
       </c>
@@ -7982,7 +7983,7 @@
       </c>
       <c r="N54" s="28">
         <f t="shared" ref="N54:N58" ca="1" si="29">$M$9-M54</f>
-        <v>-51</v>
+        <v>-50</v>
       </c>
       <c r="O54" s="27">
         <v>0.44709700000000002</v>
@@ -8000,7 +8001,7 @@
         <v>1.6871973902345887</v>
       </c>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:21">
       <c r="B55" s="1">
         <v>44729</v>
       </c>
@@ -8042,7 +8043,7 @@
       </c>
       <c r="N55" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-37</v>
+        <v>-36</v>
       </c>
       <c r="O55" s="27">
         <v>7.9225000000000004E-2</v>
@@ -8060,7 +8061,7 @@
         <v>1.1474438584033493</v>
       </c>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:21">
       <c r="B56" s="1">
         <v>44729</v>
       </c>
@@ -8102,7 +8103,7 @@
       </c>
       <c r="N56" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-23</v>
+        <v>-22</v>
       </c>
       <c r="O56" s="27">
         <v>4.7683999999999997E-2</v>
@@ -8120,7 +8121,7 @@
         <v>1.122799979907529</v>
       </c>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:21">
       <c r="B57" s="1">
         <v>44729</v>
       </c>
@@ -8162,7 +8163,7 @@
       </c>
       <c r="N57" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-16</v>
+        <v>-15</v>
       </c>
       <c r="O57" s="27">
         <v>3.1424000000000001E-2</v>
@@ -8180,7 +8181,7 @@
         <v>1.0995310894115367</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:21">
       <c r="B58" s="1">
         <v>44730</v>
       </c>
@@ -8222,7 +8223,7 @@
       </c>
       <c r="N58" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-23</v>
+        <v>-22</v>
       </c>
       <c r="O58" s="32">
         <v>2.7649E-2</v>
@@ -8240,7 +8241,7 @@
         <v>1.0721858084819609</v>
       </c>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:21">
       <c r="A59">
         <v>202</v>
       </c>
@@ -8282,7 +8283,7 @@
       </c>
       <c r="N59" s="28">
         <f ca="1">$M$9-M59</f>
-        <v>-39</v>
+        <v>-38</v>
       </c>
       <c r="O59">
         <v>6.7000000000000004E-2</v>
@@ -8300,7 +8301,7 @@
         <v>1.1323529188332864</v>
       </c>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60" spans="1:21">
       <c r="A60">
         <v>37</v>
       </c>
@@ -8342,7 +8343,7 @@
       </c>
       <c r="N60" s="28">
         <f ca="1">$M$9-M60</f>
-        <v>-25</v>
+        <v>-24</v>
       </c>
       <c r="O60">
         <v>0.08</v>
@@ -8359,8 +8360,14 @@
         <f>(1+Q60)^92</f>
         <v>1.2315179609375255</v>
       </c>
-    </row>
-    <row r="61" spans="1:18">
+      <c r="T60" s="39">
+        <v>0.13</v>
+      </c>
+      <c r="U60" s="1">
+        <v>44778</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21">
       <c r="B61" s="1">
         <v>44741</v>
       </c>
@@ -8402,7 +8409,7 @@
       </c>
       <c r="N61" s="28">
         <f ca="1">$M$9-M61</f>
-        <v>-95</v>
+        <v>-94</v>
       </c>
       <c r="O61">
         <v>0.09</v>
@@ -8420,7 +8427,7 @@
         <v>1.0851687956828595</v>
       </c>
     </row>
-    <row r="62" spans="1:18">
+    <row r="62" spans="1:21">
       <c r="B62" s="1">
         <v>44743</v>
       </c>
@@ -8462,7 +8469,7 @@
       </c>
       <c r="N62" s="28">
         <f ca="1">$M$9-M62</f>
-        <v>-97</v>
+        <v>-96</v>
       </c>
       <c r="O62" s="34">
         <v>0.09</v>

</xml_diff>

<commit_message>
added some error checking for ets
gis and tvty was failing on pi_lower/pi_upper ets forecasts
</commit_message>
<xml_diff>
--- a/code/Screener/record.xlsx
+++ b/code/Screener/record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEB47A8-0FC5-4BBC-9F74-8D5F1EFEEB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149E24AF-28D7-4966-B5AA-BBBA01DFDA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="2775" windowWidth="20730" windowHeight="11835" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
+    <workbookView xWindow="4470" yWindow="2820" windowWidth="20730" windowHeight="11835" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
   <sheets>
     <sheet name="Record book" sheetId="1" r:id="rId1"/>
@@ -5725,7 +5725,7 @@
   <dimension ref="A9:U62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U61" sqref="U61"/>
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5735,6 +5735,7 @@
     <col min="6" max="6" width="9.140625" style="19"/>
     <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.7109375" style="27" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="1:18">
@@ -5748,7 +5749,7 @@
       </c>
       <c r="M9" s="1">
         <f ca="1">TODAY()</f>
-        <v>44744</v>
+        <v>44745</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>1061</v>
@@ -6247,7 +6248,7 @@
       </c>
       <c r="N24" s="28">
         <f ca="1">$M$9-M24</f>
-        <v>-19</v>
+        <v>-18</v>
       </c>
     </row>
     <row r="25" spans="2:18">
@@ -6289,7 +6290,7 @@
       </c>
       <c r="N25" s="28">
         <f ca="1">$M$9-M25</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="26" spans="2:18">
@@ -6334,7 +6335,7 @@
       </c>
       <c r="N26" s="28">
         <f t="shared" ref="N26:N51" ca="1" si="5">$M$9-M26</f>
-        <v>-64</v>
+        <v>-63</v>
       </c>
       <c r="O26">
         <v>0.1</v>
@@ -6393,7 +6394,7 @@
       </c>
       <c r="N27" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-22</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="28" spans="2:18">
@@ -6438,7 +6439,7 @@
       </c>
       <c r="N28" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-22</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="29" spans="2:18">
@@ -6483,7 +6484,7 @@
       </c>
       <c r="N29" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O29">
         <v>0.41</v>
@@ -6543,7 +6544,7 @@
       </c>
       <c r="N30" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-43</v>
+        <v>-42</v>
       </c>
       <c r="O30">
         <v>0.13400000000000001</v>
@@ -6603,7 +6604,7 @@
       </c>
       <c r="N31" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-57</v>
+        <v>-56</v>
       </c>
       <c r="O31">
         <v>0.17</v>
@@ -6663,7 +6664,7 @@
       </c>
       <c r="N32" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-57</v>
+        <v>-56</v>
       </c>
       <c r="O32">
         <v>0.12</v>
@@ -6723,7 +6724,7 @@
       </c>
       <c r="N33" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-57</v>
+        <v>-56</v>
       </c>
       <c r="O33">
         <v>0.13200000000000001</v>
@@ -6783,7 +6784,7 @@
       </c>
       <c r="N34" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-22</v>
+        <v>-21</v>
       </c>
       <c r="O34">
         <v>9.9000000000000005E-2</v>
@@ -6843,7 +6844,7 @@
       </c>
       <c r="N35" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O35">
         <v>0.12</v>
@@ -6903,7 +6904,7 @@
       </c>
       <c r="N36" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O36">
         <v>0.14000000000000001</v>
@@ -6963,7 +6964,7 @@
       </c>
       <c r="N37" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O37">
         <v>0.35</v>
@@ -7023,7 +7024,7 @@
       </c>
       <c r="N38" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O38" s="18">
         <v>0.28000000000000003</v>
@@ -7083,7 +7084,7 @@
       </c>
       <c r="N39" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="O39">
         <v>0.11</v>
@@ -7143,7 +7144,7 @@
       </c>
       <c r="N40" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O40" s="18">
         <v>0.11</v>
@@ -7203,7 +7204,7 @@
       </c>
       <c r="N41" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O41">
         <v>9.6000000000000002E-2</v>
@@ -7263,7 +7264,7 @@
       </c>
       <c r="N42" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O42">
         <v>0.22</v>
@@ -7323,7 +7324,7 @@
       </c>
       <c r="N43" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O43">
         <v>0.73</v>
@@ -7383,7 +7384,7 @@
       </c>
       <c r="N44" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O44" s="18">
         <v>0.26500000000000001</v>
@@ -7443,7 +7444,7 @@
       </c>
       <c r="N45" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O45">
         <v>0.13</v>
@@ -7503,7 +7504,7 @@
       </c>
       <c r="N46" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O46">
         <v>0.16</v>
@@ -7563,7 +7564,7 @@
       </c>
       <c r="N47" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O47" s="18">
         <v>0.09</v>
@@ -7623,7 +7624,7 @@
       </c>
       <c r="N48" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O48" s="18">
         <v>0.3</v>
@@ -7683,7 +7684,7 @@
       </c>
       <c r="N49" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-57</v>
+        <v>-56</v>
       </c>
       <c r="O49">
         <v>0.12</v>
@@ -7743,7 +7744,7 @@
       </c>
       <c r="N50" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-36</v>
+        <v>-35</v>
       </c>
       <c r="O50">
         <v>9.4899999999999998E-2</v>
@@ -7803,7 +7804,7 @@
       </c>
       <c r="N51" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="O51">
         <v>0.14000000000000001</v>
@@ -7863,7 +7864,7 @@
       </c>
       <c r="N52" s="28">
         <f t="shared" ref="N52" ca="1" si="21">$M$9-M52</f>
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="O52" s="27">
         <v>0.16561899999999999</v>
@@ -7923,7 +7924,7 @@
       </c>
       <c r="N53" s="28">
         <f t="shared" ref="N53" ca="1" si="25">$M$9-M53</f>
-        <v>-78</v>
+        <v>-77</v>
       </c>
       <c r="O53" s="27">
         <v>0.44709700000000002</v>
@@ -7983,7 +7984,7 @@
       </c>
       <c r="N54" s="28">
         <f t="shared" ref="N54:N58" ca="1" si="29">$M$9-M54</f>
-        <v>-50</v>
+        <v>-49</v>
       </c>
       <c r="O54" s="27">
         <v>0.44709700000000002</v>
@@ -8043,7 +8044,7 @@
       </c>
       <c r="N55" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-36</v>
+        <v>-35</v>
       </c>
       <c r="O55" s="27">
         <v>7.9225000000000004E-2</v>
@@ -8103,7 +8104,7 @@
       </c>
       <c r="N56" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-22</v>
+        <v>-21</v>
       </c>
       <c r="O56" s="27">
         <v>4.7683999999999997E-2</v>
@@ -8163,7 +8164,7 @@
       </c>
       <c r="N57" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-15</v>
+        <v>-14</v>
       </c>
       <c r="O57" s="27">
         <v>3.1424000000000001E-2</v>
@@ -8223,7 +8224,7 @@
       </c>
       <c r="N58" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-22</v>
+        <v>-21</v>
       </c>
       <c r="O58" s="32">
         <v>2.7649E-2</v>
@@ -8283,7 +8284,7 @@
       </c>
       <c r="N59" s="28">
         <f ca="1">$M$9-M59</f>
-        <v>-38</v>
+        <v>-37</v>
       </c>
       <c r="O59">
         <v>6.7000000000000004E-2</v>
@@ -8300,6 +8301,12 @@
         <f>(1+Q59)^92</f>
         <v>1.1323529188332864</v>
       </c>
+      <c r="T59" s="39">
+        <v>0.13</v>
+      </c>
+      <c r="U59" s="1">
+        <v>44778</v>
+      </c>
     </row>
     <row r="60" spans="1:21">
       <c r="A60">
@@ -8343,7 +8350,7 @@
       </c>
       <c r="N60" s="28">
         <f ca="1">$M$9-M60</f>
-        <v>-24</v>
+        <v>-23</v>
       </c>
       <c r="O60">
         <v>0.08</v>
@@ -8360,11 +8367,11 @@
         <f>(1+Q60)^92</f>
         <v>1.2315179609375255</v>
       </c>
-      <c r="T60" s="39">
-        <v>0.13</v>
+      <c r="T60">
+        <v>0.02</v>
       </c>
       <c r="U60" s="1">
-        <v>44778</v>
+        <v>44834</v>
       </c>
     </row>
     <row r="61" spans="1:21">
@@ -8409,7 +8416,7 @@
       </c>
       <c r="N61" s="28">
         <f ca="1">$M$9-M61</f>
-        <v>-94</v>
+        <v>-93</v>
       </c>
       <c r="O61">
         <v>0.09</v>
@@ -8469,7 +8476,7 @@
       </c>
       <c r="N62" s="28">
         <f ca="1">$M$9-M62</f>
-        <v>-96</v>
+        <v>-95</v>
       </c>
       <c r="O62" s="34">
         <v>0.09</v>

</xml_diff>

<commit_message>
added rotating plots to fred data for analyzesp1500
</commit_message>
<xml_diff>
--- a/code/Screener/record.xlsx
+++ b/code/Screener/record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149E24AF-28D7-4966-B5AA-BBBA01DFDA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9AA3B7-C27A-47E6-8557-104A7B51A84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="2820" windowWidth="20730" windowHeight="11835" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
   <sheets>
     <sheet name="Record book" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="1126">
   <si>
     <t>EXC</t>
   </si>
@@ -3447,6 +3447,9 @@
   </si>
   <si>
     <t>yea</t>
+  </si>
+  <si>
+    <t>CHEF</t>
   </si>
 </sst>
 </file>
@@ -3553,7 +3556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3631,6 +3634,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3638,10 +3646,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5722,10 +5726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EC1B12-8D19-48E1-AE18-CC4CE60CD15C}">
-  <dimension ref="A9:U62"/>
+  <dimension ref="A9:U63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V55" sqref="V55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5749,7 +5753,7 @@
       </c>
       <c r="M9" s="1">
         <f ca="1">TODAY()</f>
-        <v>44745</v>
+        <v>44746</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>1061</v>
@@ -6248,7 +6252,7 @@
       </c>
       <c r="N24" s="28">
         <f ca="1">$M$9-M24</f>
-        <v>-18</v>
+        <v>-17</v>
       </c>
     </row>
     <row r="25" spans="2:18">
@@ -6290,7 +6294,7 @@
       </c>
       <c r="N25" s="28">
         <f ca="1">$M$9-M25</f>
-        <v>-4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="26" spans="2:18">
@@ -6335,7 +6339,7 @@
       </c>
       <c r="N26" s="28">
         <f t="shared" ref="N26:N51" ca="1" si="5">$M$9-M26</f>
-        <v>-63</v>
+        <v>-62</v>
       </c>
       <c r="O26">
         <v>0.1</v>
@@ -6394,7 +6398,7 @@
       </c>
       <c r="N27" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-21</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="28" spans="2:18">
@@ -6439,7 +6443,7 @@
       </c>
       <c r="N28" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-21</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="29" spans="2:18">
@@ -6484,7 +6488,7 @@
       </c>
       <c r="N29" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O29">
         <v>0.41</v>
@@ -6544,7 +6548,7 @@
       </c>
       <c r="N30" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-42</v>
+        <v>-41</v>
       </c>
       <c r="O30">
         <v>0.13400000000000001</v>
@@ -6604,7 +6608,7 @@
       </c>
       <c r="N31" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-56</v>
+        <v>-55</v>
       </c>
       <c r="O31">
         <v>0.17</v>
@@ -6664,7 +6668,7 @@
       </c>
       <c r="N32" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-56</v>
+        <v>-55</v>
       </c>
       <c r="O32">
         <v>0.12</v>
@@ -6724,7 +6728,7 @@
       </c>
       <c r="N33" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-56</v>
+        <v>-55</v>
       </c>
       <c r="O33">
         <v>0.13200000000000001</v>
@@ -6784,7 +6788,7 @@
       </c>
       <c r="N34" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-21</v>
+        <v>-20</v>
       </c>
       <c r="O34">
         <v>9.9000000000000005E-2</v>
@@ -6844,7 +6848,7 @@
       </c>
       <c r="N35" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O35">
         <v>0.12</v>
@@ -6904,7 +6908,7 @@
       </c>
       <c r="N36" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O36">
         <v>0.14000000000000001</v>
@@ -6964,7 +6968,7 @@
       </c>
       <c r="N37" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O37">
         <v>0.35</v>
@@ -7024,7 +7028,7 @@
       </c>
       <c r="N38" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O38" s="18">
         <v>0.28000000000000003</v>
@@ -7084,7 +7088,7 @@
       </c>
       <c r="N39" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O39">
         <v>0.11</v>
@@ -7144,7 +7148,7 @@
       </c>
       <c r="N40" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O40" s="18">
         <v>0.11</v>
@@ -7204,7 +7208,7 @@
       </c>
       <c r="N41" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O41">
         <v>9.6000000000000002E-2</v>
@@ -7264,7 +7268,7 @@
       </c>
       <c r="N42" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O42">
         <v>0.22</v>
@@ -7324,7 +7328,7 @@
       </c>
       <c r="N43" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O43">
         <v>0.73</v>
@@ -7384,7 +7388,7 @@
       </c>
       <c r="N44" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O44" s="18">
         <v>0.26500000000000001</v>
@@ -7444,7 +7448,7 @@
       </c>
       <c r="N45" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O45">
         <v>0.13</v>
@@ -7504,7 +7508,7 @@
       </c>
       <c r="N46" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O46">
         <v>0.16</v>
@@ -7564,7 +7568,7 @@
       </c>
       <c r="N47" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O47" s="18">
         <v>0.09</v>
@@ -7624,7 +7628,7 @@
       </c>
       <c r="N48" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O48" s="18">
         <v>0.3</v>
@@ -7684,7 +7688,7 @@
       </c>
       <c r="N49" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-56</v>
+        <v>-55</v>
       </c>
       <c r="O49">
         <v>0.12</v>
@@ -7744,7 +7748,7 @@
       </c>
       <c r="N50" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-35</v>
+        <v>-34</v>
       </c>
       <c r="O50">
         <v>9.4899999999999998E-2</v>
@@ -7804,7 +7808,7 @@
       </c>
       <c r="N51" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="O51">
         <v>0.14000000000000001</v>
@@ -7864,7 +7868,7 @@
       </c>
       <c r="N52" s="28">
         <f t="shared" ref="N52" ca="1" si="21">$M$9-M52</f>
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="O52" s="27">
         <v>0.16561899999999999</v>
@@ -7924,7 +7928,7 @@
       </c>
       <c r="N53" s="28">
         <f t="shared" ref="N53" ca="1" si="25">$M$9-M53</f>
-        <v>-77</v>
+        <v>-76</v>
       </c>
       <c r="O53" s="27">
         <v>0.44709700000000002</v>
@@ -7984,7 +7988,7 @@
       </c>
       <c r="N54" s="28">
         <f t="shared" ref="N54:N58" ca="1" si="29">$M$9-M54</f>
-        <v>-49</v>
+        <v>-48</v>
       </c>
       <c r="O54" s="27">
         <v>0.44709700000000002</v>
@@ -8044,7 +8048,7 @@
       </c>
       <c r="N55" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-35</v>
+        <v>-34</v>
       </c>
       <c r="O55" s="27">
         <v>7.9225000000000004E-2</v>
@@ -8104,7 +8108,7 @@
       </c>
       <c r="N56" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-21</v>
+        <v>-20</v>
       </c>
       <c r="O56" s="27">
         <v>4.7683999999999997E-2</v>
@@ -8164,7 +8168,7 @@
       </c>
       <c r="N57" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-14</v>
+        <v>-13</v>
       </c>
       <c r="O57" s="27">
         <v>3.1424000000000001E-2</v>
@@ -8224,7 +8228,7 @@
       </c>
       <c r="N58" s="28">
         <f t="shared" ca="1" si="29"/>
-        <v>-21</v>
+        <v>-20</v>
       </c>
       <c r="O58" s="32">
         <v>2.7649E-2</v>
@@ -8284,7 +8288,7 @@
       </c>
       <c r="N59" s="28">
         <f ca="1">$M$9-M59</f>
-        <v>-37</v>
+        <v>-36</v>
       </c>
       <c r="O59">
         <v>6.7000000000000004E-2</v>
@@ -8301,7 +8305,7 @@
         <f>(1+Q59)^92</f>
         <v>1.1323529188332864</v>
       </c>
-      <c r="T59" s="39">
+      <c r="T59" s="37">
         <v>0.13</v>
       </c>
       <c r="U59" s="1">
@@ -8350,7 +8354,7 @@
       </c>
       <c r="N60" s="28">
         <f ca="1">$M$9-M60</f>
-        <v>-23</v>
+        <v>-22</v>
       </c>
       <c r="O60">
         <v>0.08</v>
@@ -8416,7 +8420,7 @@
       </c>
       <c r="N61" s="28">
         <f ca="1">$M$9-M61</f>
-        <v>-93</v>
+        <v>-92</v>
       </c>
       <c r="O61">
         <v>0.09</v>
@@ -8471,12 +8475,12 @@
       <c r="L62" t="s">
         <v>142</v>
       </c>
-      <c r="M62" s="38">
+      <c r="M62" s="36">
         <v>44840</v>
       </c>
       <c r="N62" s="28">
         <f ca="1">$M$9-M62</f>
-        <v>-95</v>
+        <v>-94</v>
       </c>
       <c r="O62" s="34">
         <v>0.09</v>
@@ -8494,13 +8498,72 @@
         <v>1.0851687956828595</v>
       </c>
     </row>
+    <row r="63" spans="1:21">
+      <c r="B63" s="1">
+        <v>44744</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D63" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>37</v>
+      </c>
+      <c r="F63" s="19">
+        <v>39.4</v>
+      </c>
+      <c r="G63" s="35">
+        <v>31.5</v>
+      </c>
+      <c r="H63" s="35">
+        <f>G63*E63</f>
+        <v>1165.5</v>
+      </c>
+      <c r="I63" s="35">
+        <v>-1</v>
+      </c>
+      <c r="J63" s="35">
+        <f t="shared" ref="J63" si="48">I63*H63</f>
+        <v>-1165.5</v>
+      </c>
+      <c r="K63" t="s">
+        <v>1100</v>
+      </c>
+      <c r="L63" t="s">
+        <v>142</v>
+      </c>
+      <c r="M63" s="1">
+        <v>44834</v>
+      </c>
+      <c r="N63" s="28">
+        <f ca="1">$M$9-M63</f>
+        <v>-88</v>
+      </c>
+      <c r="O63">
+        <v>0.19</v>
+      </c>
+      <c r="P63" s="35">
+        <f>M63-B63</f>
+        <v>90</v>
+      </c>
+      <c r="Q63" s="35">
+        <f>(1+O63)^(1/P63)-1</f>
+        <v>1.9346836135925027E-3</v>
+      </c>
+      <c r="R63" s="35">
+        <f>(1+Q63)^92</f>
+        <v>1.1946090011711641</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="N24:N62">
+  <conditionalFormatting sqref="N24:N63">
     <cfRule type="expression" priority="2">
       <formula>"&gt;=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q26:Q62">
+  <conditionalFormatting sqref="Q26:Q63">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -8512,7 +8575,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P26:P62">
+  <conditionalFormatting sqref="P26:P63">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -8772,10 +8835,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="36"/>
+      <c r="B35" s="39"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -8832,10 +8895,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="36"/>
+      <c r="B44" s="39"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -9321,10 +9384,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="36"/>
+      <c r="B38" s="39"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6"/>
@@ -9381,10 +9444,10 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="36"/>
+      <c r="B47" s="39"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6"/>
@@ -10767,10 +10830,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="36"/>
+      <c r="B38" s="39"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="6"/>
@@ -10827,10 +10890,10 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="36"/>
+      <c r="B47" s="39"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="6"/>
@@ -11153,10 +11216,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="36"/>
+      <c r="B35" s="39"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -11213,10 +11276,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="36"/>
+      <c r="B44" s="39"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -11713,10 +11776,10 @@
       <c r="A14" s="10"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="36"/>
+      <c r="B15" s="39"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6"/>
@@ -11773,10 +11836,10 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="36"/>
+      <c r="B24" s="39"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6"/>
@@ -12091,10 +12154,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="36"/>
+      <c r="B32" s="39"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -12151,10 +12214,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="36"/>
+      <c r="B41" s="39"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -15885,10 +15948,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="36"/>
+      <c r="B35" s="39"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -15945,10 +16008,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="36"/>
+      <c r="B44" s="39"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -16276,10 +16339,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="36"/>
+      <c r="B35" s="39"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -16336,10 +16399,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="36"/>
+      <c r="B44" s="39"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -17479,10 +17542,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="36"/>
+      <c r="B35" s="39"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -17539,10 +17602,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="36"/>
+      <c r="B44" s="39"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -18155,10 +18218,10 @@
       <c r="A62" s="10"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="35" t="s">
+      <c r="A63" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="36"/>
+      <c r="B63" s="39"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6"/>
@@ -18215,10 +18278,10 @@
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="35" t="s">
+      <c r="A72" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B72" s="36"/>
+      <c r="B72" s="39"/>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="6"/>
@@ -18678,10 +18741,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="36"/>
+      <c r="B32" s="39"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -18738,10 +18801,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="36"/>
+      <c r="B41" s="39"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -19829,10 +19892,10 @@
       <c r="A31" s="22"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="36"/>
+      <c r="B32" s="39"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="12"/>
@@ -19889,10 +19952,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="36"/>
+      <c r="B41" s="39"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="12"/>

</xml_diff>

<commit_message>
v10.3.2 added index dict lookup
</commit_message>
<xml_diff>
--- a/code/Screener/record.xlsx
+++ b/code/Screener/record.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9AA3B7-C27A-47E6-8557-104A7B51A84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF9C789-B127-4536-B60E-CC41BE4BFFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="1126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="1127">
   <si>
     <t>EXC</t>
   </si>
@@ -3450,6 +3450,9 @@
   </si>
   <si>
     <t>CHEF</t>
+  </si>
+  <si>
+    <t>NOC</t>
   </si>
 </sst>
 </file>
@@ -3556,7 +3559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3639,6 +3642,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5726,10 +5730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EC1B12-8D19-48E1-AE18-CC4CE60CD15C}">
-  <dimension ref="A9:U63"/>
+  <dimension ref="A9:U64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V55" sqref="V55"/>
+      <selection activeCell="Q66" sqref="Q66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8500,7 +8504,7 @@
     </row>
     <row r="63" spans="1:21">
       <c r="B63" s="1">
-        <v>44744</v>
+        <v>44746</v>
       </c>
       <c r="C63" t="s">
         <v>1125</v>
@@ -8546,24 +8550,83 @@
       </c>
       <c r="P63" s="35">
         <f>M63-B63</f>
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q63" s="35">
         <f>(1+O63)^(1/P63)-1</f>
-        <v>1.9346836135925027E-3</v>
+        <v>1.9786971691126976E-3</v>
       </c>
       <c r="R63" s="35">
         <f>(1+Q63)^92</f>
-        <v>1.1946090011711641</v>
+        <v>1.1994465902506755</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21">
+      <c r="B64" s="1">
+        <v>44746</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D64" t="s">
+        <v>2</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64" s="19">
+        <v>486.85</v>
+      </c>
+      <c r="G64" s="38">
+        <v>31.5</v>
+      </c>
+      <c r="H64" s="38">
+        <f>G64*E64</f>
+        <v>63</v>
+      </c>
+      <c r="I64" s="38">
+        <v>-1</v>
+      </c>
+      <c r="J64" s="38">
+        <f t="shared" ref="J64" si="49">I64*H64</f>
+        <v>-63</v>
+      </c>
+      <c r="K64" t="s">
+        <v>1064</v>
+      </c>
+      <c r="L64" t="s">
+        <v>141</v>
+      </c>
+      <c r="M64" s="1">
+        <v>44827</v>
+      </c>
+      <c r="N64" s="28">
+        <f ca="1">$M$9-M64</f>
+        <v>-81</v>
+      </c>
+      <c r="O64" s="38">
+        <v>0.19</v>
+      </c>
+      <c r="P64" s="38">
+        <f>M64-B64</f>
+        <v>81</v>
+      </c>
+      <c r="Q64" s="38">
+        <f>(1+O64)^(1/P64)-1</f>
+        <v>2.1498793766463464E-3</v>
+      </c>
+      <c r="R64" s="38">
+        <f>(1+Q64)^92</f>
+        <v>1.2184463892045581</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="N24:N63">
+  <conditionalFormatting sqref="N24:N64">
     <cfRule type="expression" priority="2">
       <formula>"&gt;=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q26:Q63">
+  <conditionalFormatting sqref="Q26:Q64">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -8575,7 +8638,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P26:P63">
+  <conditionalFormatting sqref="P26:P64">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -8835,10 +8898,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="39"/>
+      <c r="B35" s="40"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -8895,10 +8958,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="39"/>
+      <c r="B44" s="40"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -9384,10 +9447,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="39"/>
+      <c r="B38" s="40"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6"/>
@@ -9444,10 +9507,10 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="39"/>
+      <c r="B47" s="40"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6"/>
@@ -10830,10 +10893,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="39"/>
+      <c r="B38" s="40"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="6"/>
@@ -10890,10 +10953,10 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="39"/>
+      <c r="B47" s="40"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="6"/>
@@ -11216,10 +11279,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="39"/>
+      <c r="B35" s="40"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -11276,10 +11339,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="39"/>
+      <c r="B44" s="40"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -11776,10 +11839,10 @@
       <c r="A14" s="10"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="39"/>
+      <c r="B15" s="40"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6"/>
@@ -11836,10 +11899,10 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="39"/>
+      <c r="B24" s="40"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6"/>
@@ -12154,10 +12217,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="39"/>
+      <c r="B32" s="40"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -12214,10 +12277,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="39"/>
+      <c r="B41" s="40"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -15948,10 +16011,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="39"/>
+      <c r="B35" s="40"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -16008,10 +16071,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="39"/>
+      <c r="B44" s="40"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -16339,10 +16402,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="39"/>
+      <c r="B35" s="40"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -16399,10 +16462,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="39"/>
+      <c r="B44" s="40"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -17542,10 +17605,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="39"/>
+      <c r="B35" s="40"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -17602,10 +17665,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="39"/>
+      <c r="B44" s="40"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -18218,10 +18281,10 @@
       <c r="A62" s="10"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="38" t="s">
+      <c r="A63" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="39"/>
+      <c r="B63" s="40"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6"/>
@@ -18278,10 +18341,10 @@
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="38" t="s">
+      <c r="A72" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="B72" s="39"/>
+      <c r="B72" s="40"/>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="6"/>
@@ -18741,10 +18804,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="39"/>
+      <c r="B32" s="40"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -18801,10 +18864,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="39"/>
+      <c r="B41" s="40"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -19892,10 +19955,10 @@
       <c r="A31" s="22"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="39"/>
+      <c r="B32" s="40"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="12"/>
@@ -19952,10 +20015,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="40" t="s">
+      <c r="A41" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="39"/>
+      <c r="B41" s="40"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="12"/>

</xml_diff>